<commit_message>
Added a spreadsheet to document the room IDs
</commit_message>
<xml_diff>
--- a/SMB1/Research Docs/Level Offsets.xlsx
+++ b/SMB1/Research Docs/Level Offsets.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="864" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="864"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -880,33 +879,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -918,7 +898,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -926,2905 +906,3137 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD65536"/>
+  <dimension ref="A1:AD44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H2:H40"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.76530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.76530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.8520408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.9591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.55102040816327"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.0510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.1581632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.7244897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.8418367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="7.76530612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="21.4030612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.5102040816327"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.9285714285714"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="22.3979591836735"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.515306122449"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.10714285714286"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="21.6173469387755"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="7.76530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="11.7959183673469"/>
+    <col min="1" max="1" width="20.21875"/>
+    <col min="2" max="2" width="11.44140625"/>
+    <col min="3" max="3" width="11.5546875"/>
+    <col min="4" max="4" width="12.21875"/>
+    <col min="5" max="5" width="16"/>
+    <col min="6" max="6" width="10.33203125"/>
+    <col min="7" max="7" width="21.109375"/>
+    <col min="8" max="8" width="21.21875"/>
+    <col min="9" max="9" width="7.77734375"/>
+    <col min="10" max="10" width="21.109375"/>
+    <col min="11" max="11" width="21.21875"/>
+    <col min="12" max="12" width="7.77734375"/>
+    <col min="13" max="13" width="22.88671875"/>
+    <col min="14" max="14" width="23"/>
+    <col min="15" max="15" width="8.5546875"/>
+    <col min="16" max="16" width="19"/>
+    <col min="17" max="17" width="19.109375"/>
+    <col min="18" max="18" width="16.88671875"/>
+    <col min="19" max="19" width="20.6640625"/>
+    <col min="20" max="20" width="20.88671875"/>
+    <col min="21" max="21" width="7.77734375"/>
+    <col min="22" max="22" width="21.44140625"/>
+    <col min="23" max="23" width="21.5546875"/>
+    <col min="24" max="24" width="16.88671875"/>
+    <col min="25" max="25" width="22.44140625"/>
+    <col min="26" max="26" width="22.5546875"/>
+    <col min="27" max="27" width="8.109375"/>
+    <col min="28" max="28" width="21.6640625"/>
+    <col min="29" max="29" width="21.77734375"/>
+    <col min="30" max="30" width="7.77734375"/>
+    <col min="31" max="1025" width="11.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="3">
         <v>49</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="3">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="S2" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="U2" t="s">
         <v>34</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="V2" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="X2" t="s">
         <v>37</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Y2" t="s">
         <v>32</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AA2" t="s">
         <v>34</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AB2" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AC2" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AD2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="3">
         <v>80</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="3">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" t="s">
         <v>44</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" t="s">
         <v>41</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" t="s">
         <v>42</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="V3" t="s">
         <v>46</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="X3" t="s">
         <v>48</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" t="s">
         <v>41</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" t="s">
         <v>42</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AB3" t="s">
         <v>41</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="AC3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="3">
         <v>41</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="3">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="3">
         <v>0</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="0" t="s">
+      <c r="G4" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" t="s">
         <v>52</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P4" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" t="s">
         <v>54</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="S4" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="T4" t="s">
         <v>52</v>
       </c>
-      <c r="V4" s="0" t="s">
+      <c r="V4" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="0" t="s">
+      <c r="W4" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="0" t="s">
+      <c r="Y4" t="s">
         <v>51</v>
       </c>
-      <c r="Z4" s="0" t="s">
+      <c r="Z4" t="s">
         <v>52</v>
       </c>
-      <c r="AB4" s="0" t="s">
+      <c r="AB4" t="s">
         <v>51</v>
       </c>
-      <c r="AC4" s="0" t="s">
+      <c r="AC4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="3">
         <v>47</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="3">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="0" t="s">
+      <c r="G5" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>60</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="N5" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="P5" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" t="s">
         <v>62</v>
       </c>
-      <c r="S5" s="0" t="s">
+      <c r="S5" t="s">
         <v>59</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="T5" t="s">
         <v>60</v>
       </c>
-      <c r="V5" s="0" t="s">
+      <c r="V5" t="s">
         <v>63</v>
       </c>
-      <c r="W5" s="0" t="s">
+      <c r="W5" t="s">
         <v>64</v>
       </c>
-      <c r="Y5" s="0" t="s">
+      <c r="Y5" t="s">
         <v>59</v>
       </c>
-      <c r="Z5" s="0" t="s">
+      <c r="Z5" t="s">
         <v>60</v>
       </c>
-      <c r="AB5" s="0" t="s">
+      <c r="AB5" t="s">
         <v>59</v>
       </c>
-      <c r="AC5" s="0" t="s">
+      <c r="AC5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="3">
         <v>49</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="3">
         <v>18</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="3">
         <v>2</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="0" t="s">
+      <c r="G6" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" t="s">
         <v>67</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="N6" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="P6" t="s">
         <v>68</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" t="s">
         <v>69</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="S6" t="s">
         <v>66</v>
       </c>
-      <c r="T6" s="0" t="s">
+      <c r="T6" t="s">
         <v>67</v>
       </c>
-      <c r="V6" s="0" t="s">
+      <c r="V6" t="s">
         <v>70</v>
       </c>
-      <c r="W6" s="0" t="s">
+      <c r="W6" t="s">
         <v>71</v>
       </c>
-      <c r="Y6" s="0" t="s">
+      <c r="Y6" t="s">
         <v>66</v>
       </c>
-      <c r="Z6" s="0" t="s">
+      <c r="Z6" t="s">
         <v>67</v>
       </c>
-      <c r="AB6" s="0" t="s">
+      <c r="AB6" t="s">
         <v>66</v>
       </c>
-      <c r="AC6" s="0" t="s">
+      <c r="AC6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="3">
         <v>60</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="3">
         <v>16</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="3">
         <v>3</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="0" t="s">
+      <c r="G7" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" t="s">
         <v>75</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="M7" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="0" t="s">
+      <c r="N7" t="s">
         <v>75</v>
       </c>
-      <c r="P7" s="0" t="s">
+      <c r="P7" t="s">
         <v>76</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" t="s">
         <v>77</v>
       </c>
-      <c r="S7" s="0" t="s">
+      <c r="S7" t="s">
         <v>74</v>
       </c>
-      <c r="T7" s="0" t="s">
+      <c r="T7" t="s">
         <v>75</v>
       </c>
-      <c r="V7" s="0" t="s">
+      <c r="V7" t="s">
         <v>78</v>
       </c>
-      <c r="W7" s="0" t="s">
+      <c r="W7" t="s">
         <v>79</v>
       </c>
-      <c r="Y7" s="0" t="s">
+      <c r="Y7" t="s">
         <v>74</v>
       </c>
-      <c r="Z7" s="0" t="s">
+      <c r="Z7" t="s">
         <v>75</v>
       </c>
-      <c r="AB7" s="0" t="s">
+      <c r="AB7" t="s">
         <v>74</v>
       </c>
-      <c r="AC7" s="0" t="s">
+      <c r="AC7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="3">
         <v>65</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="3">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="3">
         <v>0</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="0" t="s">
+      <c r="G8" t="s">
         <v>82</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" t="s">
         <v>82</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" t="s">
         <v>83</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="M8" t="s">
         <v>82</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="N8" t="s">
         <v>83</v>
       </c>
-      <c r="P8" s="0" t="s">
+      <c r="P8" t="s">
         <v>84</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" t="s">
         <v>85</v>
       </c>
-      <c r="S8" s="0" t="s">
+      <c r="S8" t="s">
         <v>82</v>
       </c>
-      <c r="T8" s="0" t="s">
+      <c r="T8" t="s">
         <v>83</v>
       </c>
-      <c r="V8" s="0" t="s">
+      <c r="V8" t="s">
         <v>86</v>
       </c>
-      <c r="W8" s="0" t="s">
+      <c r="W8" t="s">
         <v>87</v>
       </c>
-      <c r="Y8" s="0" t="s">
+      <c r="Y8" t="s">
         <v>82</v>
       </c>
-      <c r="Z8" s="0" t="s">
+      <c r="Z8" t="s">
         <v>83</v>
       </c>
-      <c r="AB8" s="0" t="s">
+      <c r="AB8" t="s">
         <v>82</v>
       </c>
-      <c r="AC8" s="0" t="s">
+      <c r="AC8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="3">
         <v>56</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="3">
         <v>23</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="3">
         <v>0</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="0" t="s">
+      <c r="G9" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" t="s">
         <v>91</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="M9" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="0" t="s">
+      <c r="N9" t="s">
         <v>91</v>
       </c>
-      <c r="P9" s="0" t="s">
+      <c r="P9" t="s">
         <v>92</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" t="s">
         <v>93</v>
       </c>
-      <c r="S9" s="0" t="s">
+      <c r="S9" t="s">
         <v>90</v>
       </c>
-      <c r="T9" s="0" t="s">
+      <c r="T9" t="s">
         <v>91</v>
       </c>
-      <c r="V9" s="0" t="s">
+      <c r="V9" t="s">
         <v>94</v>
       </c>
-      <c r="W9" s="0" t="s">
+      <c r="W9" t="s">
         <v>95</v>
       </c>
-      <c r="Y9" s="0" t="s">
+      <c r="Y9" t="s">
         <v>90</v>
       </c>
-      <c r="Z9" s="0" t="s">
+      <c r="Z9" t="s">
         <v>91</v>
       </c>
-      <c r="AB9" s="0" t="s">
+      <c r="AB9" t="s">
         <v>90</v>
       </c>
-      <c r="AC9" s="0" t="s">
+      <c r="AC9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="3">
         <v>57</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="3">
         <v>21</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="3">
         <v>2</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="0" t="s">
+      <c r="G10" t="s">
         <v>97</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" t="s">
         <v>98</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" t="s">
         <v>97</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="0" t="s">
+      <c r="M10" t="s">
         <v>97</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="N10" t="s">
         <v>98</v>
       </c>
-      <c r="P10" s="0" t="s">
+      <c r="P10" t="s">
         <v>99</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" t="s">
         <v>100</v>
       </c>
-      <c r="S10" s="0" t="s">
+      <c r="S10" t="s">
         <v>97</v>
       </c>
-      <c r="T10" s="0" t="s">
+      <c r="T10" t="s">
         <v>98</v>
       </c>
-      <c r="V10" s="0" t="s">
+      <c r="V10" t="s">
         <v>101</v>
       </c>
-      <c r="W10" s="0" t="s">
+      <c r="W10" t="s">
         <v>102</v>
       </c>
-      <c r="Y10" s="0" t="s">
+      <c r="Y10" t="s">
         <v>97</v>
       </c>
-      <c r="Z10" s="0" t="s">
+      <c r="Z10" t="s">
         <v>98</v>
       </c>
-      <c r="AB10" s="0" t="s">
+      <c r="AB10" t="s">
         <v>97</v>
       </c>
-      <c r="AC10" s="0" t="s">
+      <c r="AC10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="3">
         <v>24</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="3">
         <v>18</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="0" t="s">
+      <c r="G11" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" t="s">
         <v>105</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" t="s">
         <v>104</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" t="s">
         <v>105</v>
       </c>
-      <c r="M11" s="0" t="s">
+      <c r="M11" t="s">
         <v>104</v>
       </c>
-      <c r="N11" s="0" t="s">
+      <c r="N11" t="s">
         <v>105</v>
       </c>
-      <c r="P11" s="0" t="s">
+      <c r="P11" t="s">
         <v>106</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" t="s">
         <v>107</v>
       </c>
-      <c r="S11" s="0" t="s">
+      <c r="S11" t="s">
         <v>104</v>
       </c>
-      <c r="T11" s="0" t="s">
+      <c r="T11" t="s">
         <v>105</v>
       </c>
-      <c r="V11" s="0" t="s">
+      <c r="V11" t="s">
         <v>108</v>
       </c>
-      <c r="W11" s="0" t="s">
+      <c r="W11" t="s">
         <v>109</v>
       </c>
-      <c r="Y11" s="0" t="s">
+      <c r="Y11" t="s">
         <v>104</v>
       </c>
-      <c r="Z11" s="0" t="s">
+      <c r="Z11" t="s">
         <v>105</v>
       </c>
-      <c r="AB11" s="0" t="s">
+      <c r="AB11" t="s">
         <v>104</v>
       </c>
-      <c r="AC11" s="0" t="s">
+      <c r="AC11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="3">
         <v>48</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="3">
         <v>18</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="3">
         <v>0</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="0" t="s">
+      <c r="G12" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" t="s">
         <v>111</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="K12" t="s">
         <v>112</v>
       </c>
-      <c r="M12" s="0" t="s">
+      <c r="M12" t="s">
         <v>111</v>
       </c>
-      <c r="N12" s="0" t="s">
+      <c r="N12" t="s">
         <v>112</v>
       </c>
-      <c r="P12" s="0" t="s">
+      <c r="P12" t="s">
         <v>113</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" t="s">
         <v>114</v>
       </c>
-      <c r="S12" s="0" t="s">
+      <c r="S12" t="s">
         <v>111</v>
       </c>
-      <c r="T12" s="0" t="s">
+      <c r="T12" t="s">
         <v>112</v>
       </c>
-      <c r="V12" s="0" t="s">
+      <c r="V12" t="s">
         <v>115</v>
       </c>
-      <c r="W12" s="0" t="s">
+      <c r="W12" t="s">
         <v>116</v>
       </c>
-      <c r="Y12" s="0" t="s">
+      <c r="Y12" t="s">
         <v>111</v>
       </c>
-      <c r="Z12" s="0" t="s">
+      <c r="Z12" t="s">
         <v>112</v>
       </c>
-      <c r="AB12" s="0" t="s">
+      <c r="AB12" t="s">
         <v>111</v>
       </c>
-      <c r="AC12" s="0" t="s">
+      <c r="AC12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="3">
         <v>53</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="3">
         <v>21</v>
       </c>
-      <c r="E13" s="3" t="n">
+      <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="0" t="s">
+      <c r="G13" t="s">
         <v>118</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" t="s">
         <v>119</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" t="s">
         <v>118</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="K13" t="s">
         <v>119</v>
       </c>
-      <c r="M13" s="0" t="s">
+      <c r="M13" t="s">
         <v>118</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="N13" t="s">
         <v>119</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="P13" t="s">
         <v>120</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" t="s">
         <v>121</v>
       </c>
-      <c r="S13" s="0" t="s">
+      <c r="S13" t="s">
         <v>118</v>
       </c>
-      <c r="T13" s="0" t="s">
+      <c r="T13" t="s">
         <v>119</v>
       </c>
-      <c r="V13" s="0" t="s">
+      <c r="V13" t="s">
         <v>122</v>
       </c>
-      <c r="W13" s="0" t="s">
+      <c r="W13" t="s">
         <v>123</v>
       </c>
-      <c r="Y13" s="0" t="s">
+      <c r="Y13" t="s">
         <v>118</v>
       </c>
-      <c r="Z13" s="0" t="s">
+      <c r="Z13" t="s">
         <v>119</v>
       </c>
-      <c r="AB13" s="0" t="s">
+      <c r="AB13" t="s">
         <v>118</v>
       </c>
-      <c r="AC13" s="0" t="s">
+      <c r="AC13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="3">
         <v>40</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="3">
         <v>5</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="0" t="s">
+      <c r="G14" t="s">
         <v>125</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" t="s">
         <v>126</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" t="s">
         <v>125</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" t="s">
         <v>126</v>
       </c>
-      <c r="M14" s="0" t="s">
+      <c r="M14" t="s">
         <v>125</v>
       </c>
-      <c r="N14" s="0" t="s">
+      <c r="N14" t="s">
         <v>126</v>
       </c>
-      <c r="P14" s="0" t="s">
+      <c r="P14" t="s">
         <v>127</v>
       </c>
-      <c r="Q14" s="0" t="s">
+      <c r="Q14" t="s">
         <v>128</v>
       </c>
-      <c r="S14" s="0" t="s">
+      <c r="S14" t="s">
         <v>125</v>
       </c>
-      <c r="T14" s="0" t="s">
+      <c r="T14" t="s">
         <v>126</v>
       </c>
-      <c r="V14" s="0" t="s">
+      <c r="V14" t="s">
         <v>129</v>
       </c>
-      <c r="W14" s="0" t="s">
+      <c r="W14" t="s">
         <v>130</v>
       </c>
-      <c r="Y14" s="0" t="s">
+      <c r="Y14" t="s">
         <v>125</v>
       </c>
-      <c r="Z14" s="0" t="s">
+      <c r="Z14" t="s">
         <v>126</v>
       </c>
-      <c r="AB14" s="0" t="s">
+      <c r="AB14" t="s">
         <v>125</v>
       </c>
-      <c r="AC14" s="0" t="s">
+      <c r="AC14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="3">
         <v>79</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="3">
         <v>18</v>
       </c>
-      <c r="E15" s="3" t="n">
+      <c r="E15" s="3">
         <v>3</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="0" t="s">
+      <c r="G15" t="s">
         <v>132</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" t="s">
         <v>133</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" t="s">
         <v>132</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K15" t="s">
         <v>133</v>
       </c>
-      <c r="M15" s="0" t="s">
+      <c r="M15" t="s">
         <v>132</v>
       </c>
-      <c r="N15" s="0" t="s">
+      <c r="N15" t="s">
         <v>133</v>
       </c>
-      <c r="P15" s="0" t="s">
+      <c r="P15" t="s">
         <v>134</v>
       </c>
-      <c r="Q15" s="0" t="s">
+      <c r="Q15" t="s">
         <v>135</v>
       </c>
-      <c r="S15" s="0" t="s">
+      <c r="S15" t="s">
         <v>132</v>
       </c>
-      <c r="T15" s="0" t="s">
+      <c r="T15" t="s">
         <v>133</v>
       </c>
-      <c r="V15" s="0" t="s">
+      <c r="V15" t="s">
         <v>136</v>
       </c>
-      <c r="W15" s="0" t="s">
+      <c r="W15" t="s">
         <v>137</v>
       </c>
-      <c r="Y15" s="0" t="s">
+      <c r="Y15" t="s">
         <v>132</v>
       </c>
-      <c r="Z15" s="0" t="s">
+      <c r="Z15" t="s">
         <v>133</v>
       </c>
-      <c r="AB15" s="0" t="s">
+      <c r="AB15" t="s">
         <v>132</v>
       </c>
-      <c r="AC15" s="0" t="s">
+      <c r="AC15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="3">
         <v>50</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="3">
         <v>18</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="0" t="s">
+      <c r="G16" t="s">
         <v>139</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" t="s">
         <v>140</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" t="s">
         <v>139</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" t="s">
         <v>140</v>
       </c>
-      <c r="M16" s="0" t="s">
+      <c r="M16" t="s">
         <v>139</v>
       </c>
-      <c r="N16" s="0" t="s">
+      <c r="N16" t="s">
         <v>140</v>
       </c>
-      <c r="P16" s="0" t="s">
+      <c r="P16" t="s">
         <v>141</v>
       </c>
-      <c r="Q16" s="0" t="s">
+      <c r="Q16" t="s">
         <v>142</v>
       </c>
-      <c r="S16" s="0" t="s">
+      <c r="S16" t="s">
         <v>139</v>
       </c>
-      <c r="T16" s="0" t="s">
+      <c r="T16" t="s">
         <v>140</v>
       </c>
-      <c r="V16" s="0" t="s">
+      <c r="V16" t="s">
         <v>143</v>
       </c>
-      <c r="W16" s="0" t="s">
+      <c r="W16" t="s">
         <v>144</v>
       </c>
-      <c r="Y16" s="0" t="s">
+      <c r="Y16" t="s">
         <v>139</v>
       </c>
-      <c r="Z16" s="0" t="s">
+      <c r="Z16" t="s">
         <v>140</v>
       </c>
-      <c r="AB16" s="0" t="s">
+      <c r="AB16" t="s">
         <v>139</v>
       </c>
-      <c r="AC16" s="0" t="s">
+      <c r="AC16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="3">
         <v>62</v>
       </c>
-      <c r="D17" s="3" t="n">
+      <c r="D17" s="3">
         <v>12</v>
       </c>
-      <c r="E17" s="3" t="n">
+      <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="0" t="s">
+      <c r="G17" t="s">
         <v>146</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" t="s">
         <v>147</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" t="s">
         <v>146</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="K17" t="s">
         <v>147</v>
       </c>
-      <c r="M17" s="0" t="s">
+      <c r="M17" t="s">
         <v>146</v>
       </c>
-      <c r="N17" s="0" t="s">
+      <c r="N17" t="s">
         <v>147</v>
       </c>
-      <c r="P17" s="0" t="s">
+      <c r="P17" t="s">
         <v>148</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q17" t="s">
         <v>149</v>
       </c>
-      <c r="S17" s="0" t="s">
+      <c r="S17" t="s">
         <v>146</v>
       </c>
-      <c r="T17" s="0" t="s">
+      <c r="T17" t="s">
         <v>147</v>
       </c>
-      <c r="V17" s="0" t="s">
+      <c r="V17" t="s">
         <v>150</v>
       </c>
-      <c r="W17" s="0" t="s">
+      <c r="W17" t="s">
         <v>151</v>
       </c>
-      <c r="Y17" s="0" t="s">
+      <c r="Y17" t="s">
         <v>146</v>
       </c>
-      <c r="Z17" s="0" t="s">
+      <c r="Z17" t="s">
         <v>147</v>
       </c>
-      <c r="AB17" s="0" t="s">
+      <c r="AB17" t="s">
         <v>146</v>
       </c>
-      <c r="AC17" s="0" t="s">
+      <c r="AC17" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="3">
         <v>30</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="3">
         <v>16</v>
       </c>
-      <c r="E18" s="3" t="n">
+      <c r="E18" s="3">
         <v>1</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="0" t="s">
+      <c r="G18" t="s">
         <v>153</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" t="s">
         <v>154</v>
       </c>
-      <c r="J18" s="0" t="s">
+      <c r="J18" t="s">
         <v>153</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="K18" t="s">
         <v>154</v>
       </c>
-      <c r="M18" s="0" t="s">
+      <c r="M18" t="s">
         <v>153</v>
       </c>
-      <c r="N18" s="0" t="s">
+      <c r="N18" t="s">
         <v>154</v>
       </c>
-      <c r="P18" s="0" t="s">
+      <c r="P18" t="s">
         <v>155</v>
       </c>
-      <c r="Q18" s="0" t="s">
+      <c r="Q18" t="s">
         <v>156</v>
       </c>
-      <c r="S18" s="0" t="s">
+      <c r="S18" t="s">
         <v>153</v>
       </c>
-      <c r="T18" s="0" t="s">
+      <c r="T18" t="s">
         <v>154</v>
       </c>
-      <c r="V18" s="0" t="s">
+      <c r="V18" t="s">
         <v>157</v>
       </c>
-      <c r="W18" s="0" t="s">
+      <c r="W18" t="s">
         <v>158</v>
       </c>
-      <c r="Y18" s="0" t="s">
+      <c r="Y18" t="s">
         <v>153</v>
       </c>
-      <c r="Z18" s="0" t="s">
+      <c r="Z18" t="s">
         <v>154</v>
       </c>
-      <c r="AB18" s="0" t="s">
+      <c r="AB18" t="s">
         <v>153</v>
       </c>
-      <c r="AC18" s="0" t="s">
+      <c r="AC18" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="3">
         <v>56</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="3">
         <v>18</v>
       </c>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="3">
         <v>2</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="0" t="s">
+      <c r="G19" t="s">
         <v>160</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" t="s">
         <v>161</v>
       </c>
-      <c r="J19" s="0" t="s">
+      <c r="J19" t="s">
         <v>160</v>
       </c>
-      <c r="K19" s="0" t="s">
+      <c r="K19" t="s">
         <v>161</v>
       </c>
-      <c r="M19" s="0" t="s">
+      <c r="M19" t="s">
         <v>160</v>
       </c>
-      <c r="N19" s="0" t="s">
+      <c r="N19" t="s">
         <v>161</v>
       </c>
-      <c r="P19" s="0" t="s">
+      <c r="P19" t="s">
         <v>162</v>
       </c>
-      <c r="Q19" s="0" t="s">
+      <c r="Q19" t="s">
         <v>163</v>
       </c>
-      <c r="S19" s="0" t="s">
+      <c r="S19" t="s">
         <v>160</v>
       </c>
-      <c r="T19" s="0" t="s">
+      <c r="T19" t="s">
         <v>161</v>
       </c>
-      <c r="V19" s="0" t="s">
+      <c r="V19" t="s">
         <v>164</v>
       </c>
-      <c r="W19" s="0" t="s">
+      <c r="W19" t="s">
         <v>165</v>
       </c>
-      <c r="Y19" s="0" t="s">
+      <c r="Y19" t="s">
         <v>160</v>
       </c>
-      <c r="Z19" s="0" t="s">
+      <c r="Z19" t="s">
         <v>161</v>
       </c>
-      <c r="AB19" s="0" t="s">
+      <c r="AB19" t="s">
         <v>160</v>
       </c>
-      <c r="AC19" s="0" t="s">
+      <c r="AC19" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>167</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="3">
         <v>41</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="3">
         <v>14</v>
       </c>
-      <c r="E20" s="3" t="n">
+      <c r="E20" s="3">
         <v>0</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="0" t="s">
+      <c r="G20" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="J20" t="s">
         <v>51</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" t="s">
         <v>52</v>
       </c>
-      <c r="M20" s="0" t="s">
+      <c r="M20" t="s">
         <v>51</v>
       </c>
-      <c r="N20" s="0" t="s">
+      <c r="N20" t="s">
         <v>52</v>
       </c>
-      <c r="P20" s="0" t="s">
+      <c r="P20" t="s">
         <v>53</v>
       </c>
-      <c r="Q20" s="0" t="s">
+      <c r="Q20" t="s">
         <v>54</v>
       </c>
-      <c r="S20" s="0" t="s">
+      <c r="S20" t="s">
         <v>51</v>
       </c>
-      <c r="T20" s="0" t="s">
+      <c r="T20" t="s">
         <v>52</v>
       </c>
-      <c r="V20" s="0" t="s">
+      <c r="V20" t="s">
         <v>55</v>
       </c>
-      <c r="W20" s="0" t="s">
+      <c r="W20" t="s">
         <v>56</v>
       </c>
-      <c r="Y20" s="0" t="s">
+      <c r="Y20" t="s">
         <v>51</v>
       </c>
-      <c r="Z20" s="0" t="s">
+      <c r="Z20" t="s">
         <v>52</v>
       </c>
-      <c r="AB20" s="0" t="s">
+      <c r="AB20" t="s">
         <v>51</v>
       </c>
-      <c r="AC20" s="0" t="s">
+      <c r="AC20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>169</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="3">
         <v>56</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="3">
         <v>23</v>
       </c>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="0" t="s">
+      <c r="G21" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" t="s">
         <v>91</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" t="s">
         <v>90</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="K21" t="s">
         <v>91</v>
       </c>
-      <c r="M21" s="0" t="s">
+      <c r="M21" t="s">
         <v>90</v>
       </c>
-      <c r="N21" s="0" t="s">
+      <c r="N21" t="s">
         <v>91</v>
       </c>
-      <c r="P21" s="0" t="s">
+      <c r="P21" t="s">
         <v>92</v>
       </c>
-      <c r="Q21" s="0" t="s">
+      <c r="Q21" t="s">
         <v>93</v>
       </c>
-      <c r="S21" s="0" t="s">
+      <c r="S21" t="s">
         <v>90</v>
       </c>
-      <c r="T21" s="0" t="s">
+      <c r="T21" t="s">
         <v>91</v>
       </c>
-      <c r="V21" s="0" t="s">
+      <c r="V21" t="s">
         <v>94</v>
       </c>
-      <c r="W21" s="0" t="s">
+      <c r="W21" t="s">
         <v>95</v>
       </c>
-      <c r="Y21" s="0" t="s">
+      <c r="Y21" t="s">
         <v>90</v>
       </c>
-      <c r="Z21" s="0" t="s">
+      <c r="Z21" t="s">
         <v>91</v>
       </c>
-      <c r="AB21" s="0" t="s">
+      <c r="AB21" t="s">
         <v>90</v>
       </c>
-      <c r="AC21" s="0" t="s">
+      <c r="AC21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="3">
         <v>56</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="3">
         <v>4</v>
       </c>
-      <c r="E22" s="3" t="n">
+      <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="0" t="s">
+      <c r="G22" t="s">
         <v>171</v>
       </c>
-      <c r="H22" s="0" t="s">
+      <c r="H22" t="s">
         <v>172</v>
       </c>
-      <c r="J22" s="0" t="s">
+      <c r="J22" t="s">
         <v>171</v>
       </c>
-      <c r="K22" s="0" t="s">
+      <c r="K22" t="s">
         <v>172</v>
       </c>
-      <c r="M22" s="0" t="s">
+      <c r="M22" t="s">
         <v>171</v>
       </c>
-      <c r="N22" s="0" t="s">
+      <c r="N22" t="s">
         <v>172</v>
       </c>
-      <c r="P22" s="0" t="s">
+      <c r="P22" t="s">
         <v>173</v>
       </c>
-      <c r="Q22" s="0" t="s">
+      <c r="Q22" t="s">
         <v>174</v>
       </c>
-      <c r="S22" s="0" t="s">
+      <c r="S22" t="s">
         <v>171</v>
       </c>
-      <c r="T22" s="0" t="s">
+      <c r="T22" t="s">
         <v>172</v>
       </c>
-      <c r="V22" s="0" t="s">
+      <c r="V22" t="s">
         <v>175</v>
       </c>
-      <c r="W22" s="0" t="s">
+      <c r="W22" t="s">
         <v>176</v>
       </c>
-      <c r="Y22" s="0" t="s">
+      <c r="Y22" t="s">
         <v>171</v>
       </c>
-      <c r="Z22" s="0" t="s">
+      <c r="Z22" t="s">
         <v>172</v>
       </c>
-      <c r="AB22" s="0" t="s">
+      <c r="AB22" t="s">
         <v>171</v>
       </c>
-      <c r="AC22" s="0" t="s">
+      <c r="AC22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="3">
         <v>70</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="3">
         <v>13</v>
       </c>
-      <c r="E23" s="3" t="n">
+      <c r="E23" s="3">
         <v>4</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="0" t="s">
+      <c r="G23" t="s">
         <v>178</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" t="s">
         <v>179</v>
       </c>
-      <c r="J23" s="0" t="s">
+      <c r="J23" t="s">
         <v>178</v>
       </c>
-      <c r="K23" s="0" t="s">
+      <c r="K23" t="s">
         <v>179</v>
       </c>
-      <c r="M23" s="0" t="s">
+      <c r="M23" t="s">
         <v>178</v>
       </c>
-      <c r="N23" s="0" t="s">
+      <c r="N23" t="s">
         <v>179</v>
       </c>
-      <c r="P23" s="0" t="s">
+      <c r="P23" t="s">
         <v>180</v>
       </c>
-      <c r="Q23" s="0" t="s">
+      <c r="Q23" t="s">
         <v>181</v>
       </c>
-      <c r="S23" s="0" t="s">
+      <c r="S23" t="s">
         <v>178</v>
       </c>
-      <c r="T23" s="0" t="s">
+      <c r="T23" t="s">
         <v>179</v>
       </c>
-      <c r="V23" s="0" t="s">
+      <c r="V23" t="s">
         <v>182</v>
       </c>
-      <c r="W23" s="0" t="s">
+      <c r="W23" t="s">
         <v>183</v>
       </c>
-      <c r="Y23" s="0" t="s">
+      <c r="Y23" t="s">
         <v>178</v>
       </c>
-      <c r="Z23" s="0" t="s">
+      <c r="Z23" t="s">
         <v>179</v>
       </c>
-      <c r="AB23" s="0" t="s">
+      <c r="AB23" t="s">
         <v>178</v>
       </c>
-      <c r="AC23" s="0" t="s">
+      <c r="AC23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="3">
         <v>49</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="3">
         <v>17</v>
       </c>
-      <c r="E24" s="3" t="n">
+      <c r="E24" s="3">
         <v>0</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="0" t="s">
+      <c r="G24" t="s">
         <v>185</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="H24" t="s">
         <v>186</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="J24" t="s">
         <v>185</v>
       </c>
-      <c r="K24" s="0" t="s">
+      <c r="K24" t="s">
         <v>186</v>
       </c>
-      <c r="M24" s="0" t="s">
+      <c r="M24" t="s">
         <v>185</v>
       </c>
-      <c r="N24" s="0" t="s">
+      <c r="N24" t="s">
         <v>186</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="P24" t="s">
         <v>187</v>
       </c>
-      <c r="Q24" s="0" t="s">
+      <c r="Q24" t="s">
         <v>188</v>
       </c>
-      <c r="S24" s="0" t="s">
+      <c r="S24" t="s">
         <v>185</v>
       </c>
-      <c r="T24" s="0" t="s">
+      <c r="T24" t="s">
         <v>186</v>
       </c>
-      <c r="V24" s="0" t="s">
+      <c r="V24" t="s">
         <v>189</v>
       </c>
-      <c r="W24" s="0" t="s">
+      <c r="W24" t="s">
         <v>190</v>
       </c>
-      <c r="Y24" s="0" t="s">
+      <c r="Y24" t="s">
         <v>185</v>
       </c>
-      <c r="Z24" s="0" t="s">
+      <c r="Z24" t="s">
         <v>186</v>
       </c>
-      <c r="AB24" s="0" t="s">
+      <c r="AB24" t="s">
         <v>185</v>
       </c>
-      <c r="AC24" s="0" t="s">
+      <c r="AC24" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>192</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="3">
         <v>47</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="3">
         <v>19</v>
       </c>
-      <c r="E25" s="3" t="n">
+      <c r="E25" s="3">
         <v>0</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="0" t="s">
+      <c r="G25" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H25" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="J25" t="s">
         <v>59</v>
       </c>
-      <c r="K25" s="0" t="s">
+      <c r="K25" t="s">
         <v>60</v>
       </c>
-      <c r="M25" s="0" t="s">
+      <c r="M25" t="s">
         <v>59</v>
       </c>
-      <c r="N25" s="0" t="s">
+      <c r="N25" t="s">
         <v>60</v>
       </c>
-      <c r="P25" s="0" t="s">
+      <c r="P25" t="s">
         <v>61</v>
       </c>
-      <c r="Q25" s="0" t="s">
+      <c r="Q25" t="s">
         <v>62</v>
       </c>
-      <c r="S25" s="0" t="s">
+      <c r="S25" t="s">
         <v>59</v>
       </c>
-      <c r="T25" s="0" t="s">
+      <c r="T25" t="s">
         <v>60</v>
       </c>
-      <c r="V25" s="0" t="s">
+      <c r="V25" t="s">
         <v>63</v>
       </c>
-      <c r="W25" s="0" t="s">
+      <c r="W25" t="s">
         <v>64</v>
       </c>
-      <c r="Y25" s="0" t="s">
+      <c r="Y25" t="s">
         <v>59</v>
       </c>
-      <c r="Z25" s="0" t="s">
+      <c r="Z25" t="s">
         <v>60</v>
       </c>
-      <c r="AB25" s="0" t="s">
+      <c r="AB25" t="s">
         <v>59</v>
       </c>
-      <c r="AC25" s="0" t="s">
+      <c r="AC25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="3">
         <v>43</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="3">
         <v>12</v>
       </c>
-      <c r="E26" s="3" t="n">
+      <c r="E26" s="3">
         <v>1</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="0" t="s">
+      <c r="G26" t="s">
         <v>194</v>
       </c>
-      <c r="H26" s="0" t="s">
+      <c r="H26" t="s">
         <v>195</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="J26" t="s">
         <v>194</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="K26" t="s">
         <v>195</v>
       </c>
-      <c r="M26" s="0" t="s">
+      <c r="M26" t="s">
         <v>194</v>
       </c>
-      <c r="N26" s="0" t="s">
+      <c r="N26" t="s">
         <v>195</v>
       </c>
-      <c r="P26" s="0" t="s">
+      <c r="P26" t="s">
         <v>196</v>
       </c>
-      <c r="Q26" s="0" t="s">
+      <c r="Q26" t="s">
         <v>197</v>
       </c>
-      <c r="S26" s="0" t="s">
+      <c r="S26" t="s">
         <v>194</v>
       </c>
-      <c r="T26" s="0" t="s">
+      <c r="T26" t="s">
         <v>195</v>
       </c>
-      <c r="V26" s="0" t="s">
+      <c r="V26" t="s">
         <v>198</v>
       </c>
-      <c r="W26" s="0" t="s">
+      <c r="W26" t="s">
         <v>199</v>
       </c>
-      <c r="Y26" s="0" t="s">
+      <c r="Y26" t="s">
         <v>194</v>
       </c>
-      <c r="Z26" s="0" t="s">
+      <c r="Z26" t="s">
         <v>195</v>
       </c>
-      <c r="AB26" s="0" t="s">
+      <c r="AB26" t="s">
         <v>194</v>
       </c>
-      <c r="AC26" s="0" t="s">
+      <c r="AC26" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="3">
         <v>60</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="3">
         <v>20</v>
       </c>
-      <c r="E27" s="3" t="n">
+      <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="0" t="s">
+      <c r="G27" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H27" t="s">
         <v>75</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="J27" t="s">
         <v>74</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="K27" t="s">
         <v>75</v>
       </c>
-      <c r="M27" s="0" t="s">
+      <c r="M27" t="s">
         <v>74</v>
       </c>
-      <c r="N27" s="0" t="s">
+      <c r="N27" t="s">
         <v>75</v>
       </c>
-      <c r="P27" s="0" t="s">
+      <c r="P27" t="s">
         <v>76</v>
       </c>
-      <c r="Q27" s="0" t="s">
+      <c r="Q27" t="s">
         <v>77</v>
       </c>
-      <c r="S27" s="0" t="s">
+      <c r="S27" t="s">
         <v>74</v>
       </c>
-      <c r="T27" s="0" t="s">
+      <c r="T27" t="s">
         <v>75</v>
       </c>
-      <c r="V27" s="0" t="s">
+      <c r="V27" t="s">
         <v>78</v>
       </c>
-      <c r="W27" s="0" t="s">
+      <c r="W27" t="s">
         <v>79</v>
       </c>
-      <c r="Y27" s="0" t="s">
+      <c r="Y27" t="s">
         <v>74</v>
       </c>
-      <c r="Z27" s="0" t="s">
+      <c r="Z27" t="s">
         <v>75</v>
       </c>
-      <c r="AB27" s="0" t="s">
+      <c r="AB27" t="s">
         <v>74</v>
       </c>
-      <c r="AC27" s="0" t="s">
+      <c r="AC27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>203</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="3">
         <v>65</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="3">
         <v>10</v>
       </c>
-      <c r="E28" s="3" t="n">
+      <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3"/>
-      <c r="G28" s="0" t="s">
+      <c r="G28" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="0" t="s">
+      <c r="H28" t="s">
         <v>83</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="J28" t="s">
         <v>82</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="K28" t="s">
         <v>83</v>
       </c>
-      <c r="M28" s="0" t="s">
+      <c r="M28" t="s">
         <v>82</v>
       </c>
-      <c r="N28" s="0" t="s">
+      <c r="N28" t="s">
         <v>83</v>
       </c>
-      <c r="P28" s="0" t="s">
+      <c r="P28" t="s">
         <v>84</v>
       </c>
-      <c r="Q28" s="0" t="s">
+      <c r="Q28" t="s">
         <v>85</v>
       </c>
-      <c r="S28" s="0" t="s">
+      <c r="S28" t="s">
         <v>82</v>
       </c>
-      <c r="T28" s="0" t="s">
+      <c r="T28" t="s">
         <v>83</v>
       </c>
-      <c r="V28" s="0" t="s">
+      <c r="V28" t="s">
         <v>86</v>
       </c>
-      <c r="W28" s="0" t="s">
+      <c r="W28" t="s">
         <v>87</v>
       </c>
-      <c r="Y28" s="0" t="s">
+      <c r="Y28" t="s">
         <v>82</v>
       </c>
-      <c r="Z28" s="0" t="s">
+      <c r="Z28" t="s">
         <v>83</v>
       </c>
-      <c r="AB28" s="0" t="s">
+      <c r="AB28" t="s">
         <v>82</v>
       </c>
-      <c r="AC28" s="0" t="s">
+      <c r="AC28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="3">
         <v>68</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="3">
         <v>10</v>
       </c>
-      <c r="E29" s="3" t="n">
+      <c r="E29" s="3">
         <v>0</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="G29" s="0" t="s">
+      <c r="G29" t="s">
         <v>205</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="H29" t="s">
         <v>206</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" t="s">
         <v>205</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="K29" t="s">
         <v>206</v>
       </c>
-      <c r="M29" s="0" t="s">
+      <c r="M29" t="s">
         <v>205</v>
       </c>
-      <c r="N29" s="0" t="s">
+      <c r="N29" t="s">
         <v>206</v>
       </c>
-      <c r="P29" s="0" t="s">
+      <c r="P29" t="s">
         <v>207</v>
       </c>
-      <c r="Q29" s="0" t="s">
+      <c r="Q29" t="s">
         <v>208</v>
       </c>
-      <c r="S29" s="0" t="s">
+      <c r="S29" t="s">
         <v>205</v>
       </c>
-      <c r="T29" s="0" t="s">
+      <c r="T29" t="s">
         <v>206</v>
       </c>
-      <c r="V29" s="0" t="s">
+      <c r="V29" t="s">
         <v>209</v>
       </c>
-      <c r="W29" s="0" t="s">
+      <c r="W29" t="s">
         <v>210</v>
       </c>
-      <c r="Y29" s="0" t="s">
+      <c r="Y29" t="s">
         <v>205</v>
       </c>
-      <c r="Z29" s="0" t="s">
+      <c r="Z29" t="s">
         <v>206</v>
       </c>
-      <c r="AB29" s="0" t="s">
+      <c r="AB29" t="s">
         <v>205</v>
       </c>
-      <c r="AC29" s="0" t="s">
+      <c r="AC29" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="3">
         <v>72</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="3">
         <v>27</v>
       </c>
-      <c r="E30" s="3" t="n">
+      <c r="E30" s="3">
         <v>1</v>
       </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="0" t="s">
+      <c r="G30" t="s">
         <v>212</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="H30" t="s">
         <v>213</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="J30" t="s">
         <v>212</v>
       </c>
-      <c r="K30" s="0" t="s">
+      <c r="K30" t="s">
         <v>213</v>
       </c>
-      <c r="M30" s="0" t="s">
+      <c r="M30" t="s">
         <v>212</v>
       </c>
-      <c r="N30" s="0" t="s">
+      <c r="N30" t="s">
         <v>213</v>
       </c>
-      <c r="P30" s="0" t="s">
+      <c r="P30" t="s">
         <v>214</v>
       </c>
-      <c r="Q30" s="0" t="s">
+      <c r="Q30" t="s">
         <v>215</v>
       </c>
-      <c r="S30" s="0" t="s">
+      <c r="S30" t="s">
         <v>212</v>
       </c>
-      <c r="T30" s="0" t="s">
+      <c r="T30" t="s">
         <v>213</v>
       </c>
-      <c r="V30" s="0" t="s">
+      <c r="V30" t="s">
         <v>216</v>
       </c>
-      <c r="W30" s="0" t="s">
+      <c r="W30" t="s">
         <v>217</v>
       </c>
-      <c r="Y30" s="0" t="s">
+      <c r="Y30" t="s">
         <v>212</v>
       </c>
-      <c r="Z30" s="0" t="s">
+      <c r="Z30" t="s">
         <v>213</v>
       </c>
-      <c r="AB30" s="0" t="s">
+      <c r="AB30" t="s">
         <v>212</v>
       </c>
-      <c r="AC30" s="0" t="s">
+      <c r="AC30" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="3">
         <v>59</v>
       </c>
-      <c r="D31" s="3" t="n">
+      <c r="D31" s="3">
         <v>21</v>
       </c>
-      <c r="E31" s="3" t="n">
+      <c r="E31" s="3">
         <v>1</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="0" t="s">
+      <c r="G31" t="s">
         <v>219</v>
       </c>
-      <c r="H31" s="0" t="s">
+      <c r="H31" t="s">
         <v>220</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" t="s">
         <v>219</v>
       </c>
-      <c r="K31" s="0" t="s">
+      <c r="K31" t="s">
         <v>220</v>
       </c>
-      <c r="M31" s="0" t="s">
+      <c r="M31" t="s">
         <v>219</v>
       </c>
-      <c r="N31" s="0" t="s">
+      <c r="N31" t="s">
         <v>220</v>
       </c>
-      <c r="P31" s="0" t="s">
+      <c r="P31" t="s">
         <v>221</v>
       </c>
-      <c r="Q31" s="0" t="s">
+      <c r="Q31" t="s">
         <v>222</v>
       </c>
-      <c r="S31" s="0" t="s">
+      <c r="S31" t="s">
         <v>219</v>
       </c>
-      <c r="T31" s="0" t="s">
+      <c r="T31" t="s">
         <v>220</v>
       </c>
-      <c r="V31" s="0" t="s">
+      <c r="V31" t="s">
         <v>223</v>
       </c>
-      <c r="W31" s="0" t="s">
+      <c r="W31" t="s">
         <v>224</v>
       </c>
-      <c r="Y31" s="0" t="s">
+      <c r="Y31" t="s">
         <v>219</v>
       </c>
-      <c r="Z31" s="0" t="s">
+      <c r="Z31" t="s">
         <v>220</v>
       </c>
-      <c r="AB31" s="0" t="s">
+      <c r="AB31" t="s">
         <v>219</v>
       </c>
-      <c r="AC31" s="0" t="s">
+      <c r="AC31" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="3">
         <v>51</v>
       </c>
-      <c r="D32" s="3" t="n">
+      <c r="D32" s="3">
         <v>14</v>
       </c>
-      <c r="E32" s="3" t="n">
+      <c r="E32" s="3">
         <v>0</v>
       </c>
       <c r="F32" s="3"/>
-      <c r="G32" s="0" t="s">
+      <c r="G32" t="s">
         <v>226</v>
       </c>
-      <c r="H32" s="0" t="s">
+      <c r="H32" t="s">
         <v>227</v>
       </c>
-      <c r="J32" s="0" t="s">
+      <c r="J32" t="s">
         <v>226</v>
       </c>
-      <c r="K32" s="0" t="s">
+      <c r="K32" t="s">
         <v>227</v>
       </c>
-      <c r="M32" s="0" t="s">
+      <c r="M32" t="s">
         <v>226</v>
       </c>
-      <c r="N32" s="0" t="s">
+      <c r="N32" t="s">
         <v>227</v>
       </c>
-      <c r="P32" s="0" t="s">
+      <c r="P32" t="s">
         <v>228</v>
       </c>
-      <c r="Q32" s="0" t="s">
+      <c r="Q32" t="s">
         <v>229</v>
       </c>
-      <c r="S32" s="0" t="s">
+      <c r="S32" t="s">
         <v>226</v>
       </c>
-      <c r="T32" s="0" t="s">
+      <c r="T32" t="s">
         <v>227</v>
       </c>
-      <c r="V32" s="0" t="s">
+      <c r="V32" t="s">
         <v>230</v>
       </c>
-      <c r="W32" s="0" t="s">
+      <c r="W32" t="s">
         <v>231</v>
       </c>
-      <c r="Y32" s="0" t="s">
+      <c r="Y32" t="s">
         <v>226</v>
       </c>
-      <c r="Z32" s="0" t="s">
+      <c r="Z32" t="s">
         <v>227</v>
       </c>
-      <c r="AB32" s="0" t="s">
+      <c r="AB32" t="s">
         <v>226</v>
       </c>
-      <c r="AC32" s="0" t="s">
+      <c r="AC32" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="3">
         <v>55</v>
       </c>
-      <c r="D33" s="3" t="n">
+      <c r="D33" s="3">
         <v>18</v>
       </c>
-      <c r="E33" s="3" t="n">
+      <c r="E33" s="3">
         <v>7</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="0" t="s">
+      <c r="G33" t="s">
         <v>233</v>
       </c>
-      <c r="H33" s="0" t="s">
+      <c r="H33" t="s">
         <v>234</v>
       </c>
-      <c r="J33" s="0" t="s">
+      <c r="J33" t="s">
         <v>233</v>
       </c>
-      <c r="K33" s="0" t="s">
+      <c r="K33" t="s">
         <v>234</v>
       </c>
-      <c r="M33" s="0" t="s">
+      <c r="M33" t="s">
         <v>233</v>
       </c>
-      <c r="N33" s="0" t="s">
+      <c r="N33" t="s">
         <v>234</v>
       </c>
-      <c r="P33" s="0" t="s">
+      <c r="P33" t="s">
         <v>235</v>
       </c>
-      <c r="Q33" s="0" t="s">
+      <c r="Q33" t="s">
         <v>236</v>
       </c>
-      <c r="S33" s="0" t="s">
+      <c r="S33" t="s">
         <v>233</v>
       </c>
-      <c r="T33" s="0" t="s">
+      <c r="T33" t="s">
         <v>234</v>
       </c>
-      <c r="V33" s="0" t="s">
+      <c r="V33" t="s">
         <v>237</v>
       </c>
-      <c r="W33" s="0" t="s">
+      <c r="W33" t="s">
         <v>238</v>
       </c>
-      <c r="Y33" s="0" t="s">
+      <c r="Y33" t="s">
         <v>233</v>
       </c>
-      <c r="Z33" s="0" t="s">
+      <c r="Z33" t="s">
         <v>234</v>
       </c>
-      <c r="AB33" s="0" t="s">
+      <c r="AB33" t="s">
         <v>233</v>
       </c>
-      <c r="AC33" s="0" t="s">
+      <c r="AC33" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>239</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>240</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="3">
         <v>3</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" t="s">
         <v>240</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" t="s">
         <v>240</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="G34" t="s">
         <v>241</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="H34" t="s">
         <v>240</v>
       </c>
-      <c r="J34" s="0" t="s">
+      <c r="J34" t="s">
         <v>241</v>
       </c>
-      <c r="K34" s="0" t="s">
+      <c r="K34" t="s">
         <v>240</v>
       </c>
-      <c r="M34" s="0" t="s">
+      <c r="M34" t="s">
         <v>241</v>
       </c>
-      <c r="N34" s="0" t="s">
+      <c r="N34" t="s">
         <v>240</v>
       </c>
-      <c r="P34" s="0" t="s">
+      <c r="P34" t="s">
         <v>242</v>
       </c>
-      <c r="Q34" s="0" t="s">
+      <c r="Q34" t="s">
         <v>240</v>
       </c>
-      <c r="S34" s="0" t="s">
+      <c r="S34" t="s">
         <v>241</v>
       </c>
-      <c r="T34" s="0" t="s">
+      <c r="T34" t="s">
         <v>240</v>
       </c>
-      <c r="V34" s="0" t="s">
+      <c r="V34" t="s">
         <v>243</v>
       </c>
-      <c r="W34" s="0" t="s">
+      <c r="W34" t="s">
         <v>240</v>
       </c>
-      <c r="Y34" s="0" t="s">
+      <c r="Y34" t="s">
         <v>241</v>
       </c>
-      <c r="Z34" s="0" t="s">
+      <c r="Z34" t="s">
         <v>240</v>
       </c>
-      <c r="AB34" s="0" t="s">
+      <c r="AB34" t="s">
         <v>241</v>
       </c>
-      <c r="AC34" s="0" t="s">
+      <c r="AC34" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>244</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>240</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="3">
         <v>69</v>
       </c>
-      <c r="D35" s="4" t="n">
+      <c r="D35" s="4">
         <v>4</v>
       </c>
-      <c r="E35" s="4" t="n">
+      <c r="E35" s="4">
         <v>12</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="G35" t="s">
         <v>245</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="H35" t="s">
         <v>246</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="J35" t="s">
         <v>245</v>
       </c>
-      <c r="K35" s="0" t="s">
+      <c r="K35" t="s">
         <v>246</v>
       </c>
-      <c r="M35" s="0" t="s">
+      <c r="M35" t="s">
         <v>245</v>
       </c>
-      <c r="N35" s="0" t="s">
+      <c r="N35" t="s">
         <v>246</v>
       </c>
-      <c r="P35" s="0" t="s">
+      <c r="P35" t="s">
         <v>247</v>
       </c>
-      <c r="Q35" s="0" t="s">
+      <c r="Q35" t="s">
         <v>248</v>
       </c>
-      <c r="S35" s="0" t="s">
+      <c r="S35" t="s">
         <v>245</v>
       </c>
-      <c r="T35" s="0" t="s">
+      <c r="T35" t="s">
         <v>246</v>
       </c>
-      <c r="V35" s="0" t="s">
+      <c r="V35" t="s">
         <v>249</v>
       </c>
-      <c r="W35" s="0" t="s">
+      <c r="W35" t="s">
         <v>250</v>
       </c>
-      <c r="Y35" s="0" t="s">
+      <c r="Y35" t="s">
         <v>245</v>
       </c>
-      <c r="Z35" s="0" t="s">
+      <c r="Z35" t="s">
         <v>246</v>
       </c>
-      <c r="AB35" s="0" t="s">
+      <c r="AB35" t="s">
         <v>245</v>
       </c>
-      <c r="AC35" s="0" t="s">
+      <c r="AC35" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>251</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>240</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="3">
         <v>9</v>
       </c>
-      <c r="D36" s="4" t="n">
+      <c r="D36" s="4">
         <v>1</v>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="4">
         <v>2</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="G36" t="s">
         <v>252</v>
       </c>
-      <c r="H36" s="0" t="s">
+      <c r="H36" t="s">
         <v>253</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="J36" t="s">
         <v>252</v>
       </c>
-      <c r="K36" s="0" t="s">
+      <c r="K36" t="s">
         <v>253</v>
       </c>
-      <c r="M36" s="0" t="s">
+      <c r="M36" t="s">
         <v>252</v>
       </c>
-      <c r="N36" s="0" t="s">
+      <c r="N36" t="s">
         <v>253</v>
       </c>
-      <c r="P36" s="0" t="s">
+      <c r="P36" t="s">
         <v>254</v>
       </c>
-      <c r="Q36" s="0" t="s">
+      <c r="Q36" t="s">
         <v>255</v>
       </c>
-      <c r="S36" s="0" t="s">
+      <c r="S36" t="s">
         <v>252</v>
       </c>
-      <c r="T36" s="0" t="s">
+      <c r="T36" t="s">
         <v>253</v>
       </c>
-      <c r="V36" s="0" t="s">
+      <c r="V36" t="s">
         <v>256</v>
       </c>
-      <c r="W36" s="0" t="s">
+      <c r="W36" t="s">
         <v>257</v>
       </c>
-      <c r="Y36" s="0" t="s">
+      <c r="Y36" t="s">
         <v>252</v>
       </c>
-      <c r="Z36" s="0" t="s">
+      <c r="Z36" t="s">
         <v>253</v>
       </c>
-      <c r="AB36" s="0" t="s">
+      <c r="AB36" t="s">
         <v>252</v>
       </c>
-      <c r="AC36" s="0" t="s">
+      <c r="AC36" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>258</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>240</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="3">
         <v>20</v>
       </c>
-      <c r="D37" s="4" t="n">
+      <c r="D37" s="4">
         <v>1</v>
       </c>
-      <c r="E37" s="4" t="n">
+      <c r="E37" s="4">
         <v>2</v>
       </c>
-      <c r="G37" s="0" t="s">
+      <c r="G37" t="s">
         <v>259</v>
       </c>
-      <c r="H37" s="0" t="s">
+      <c r="H37" t="s">
         <v>260</v>
       </c>
-      <c r="J37" s="0" t="s">
+      <c r="J37" t="s">
         <v>259</v>
       </c>
-      <c r="K37" s="0" t="s">
+      <c r="K37" t="s">
         <v>260</v>
       </c>
-      <c r="M37" s="0" t="s">
+      <c r="M37" t="s">
         <v>259</v>
       </c>
-      <c r="N37" s="0" t="s">
+      <c r="N37" t="s">
         <v>260</v>
       </c>
-      <c r="P37" s="0" t="s">
+      <c r="P37" t="s">
         <v>261</v>
       </c>
-      <c r="Q37" s="0" t="s">
+      <c r="Q37" t="s">
         <v>262</v>
       </c>
-      <c r="S37" s="0" t="s">
+      <c r="S37" t="s">
         <v>259</v>
       </c>
-      <c r="T37" s="0" t="s">
+      <c r="T37" t="s">
         <v>260</v>
       </c>
-      <c r="V37" s="0" t="s">
+      <c r="V37" t="s">
         <v>263</v>
       </c>
-      <c r="W37" s="0" t="s">
+      <c r="W37" t="s">
         <v>264</v>
       </c>
-      <c r="Y37" s="0" t="s">
+      <c r="Y37" t="s">
         <v>259</v>
       </c>
-      <c r="Z37" s="0" t="s">
+      <c r="Z37" t="s">
         <v>260</v>
       </c>
-      <c r="AB37" s="0" t="s">
+      <c r="AB37" t="s">
         <v>259</v>
       </c>
-      <c r="AC37" s="0" t="s">
+      <c r="AC37" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>265</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>240</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="3">
         <v>23</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" t="s">
         <v>240</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" t="s">
         <v>240</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="G38" t="s">
         <v>266</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="H38" t="s">
         <v>240</v>
       </c>
-      <c r="J38" s="0" t="s">
+      <c r="J38" t="s">
         <v>266</v>
       </c>
-      <c r="K38" s="0" t="s">
+      <c r="K38" t="s">
         <v>240</v>
       </c>
-      <c r="M38" s="0" t="s">
+      <c r="M38" t="s">
         <v>266</v>
       </c>
-      <c r="N38" s="0" t="s">
+      <c r="N38" t="s">
         <v>240</v>
       </c>
-      <c r="P38" s="0" t="s">
+      <c r="P38" t="s">
         <v>267</v>
       </c>
-      <c r="Q38" s="0" t="s">
+      <c r="Q38" t="s">
         <v>240</v>
       </c>
-      <c r="S38" s="0" t="s">
+      <c r="S38" t="s">
         <v>266</v>
       </c>
-      <c r="T38" s="0" t="s">
+      <c r="T38" t="s">
         <v>240</v>
       </c>
-      <c r="V38" s="0" t="s">
+      <c r="V38" t="s">
         <v>268</v>
       </c>
-      <c r="W38" s="0" t="s">
+      <c r="W38" t="s">
         <v>240</v>
       </c>
-      <c r="Y38" s="0" t="s">
+      <c r="Y38" t="s">
         <v>266</v>
       </c>
-      <c r="Z38" s="0" t="s">
+      <c r="Z38" t="s">
         <v>240</v>
       </c>
-      <c r="AB38" s="0" t="s">
+      <c r="AB38" t="s">
         <v>266</v>
       </c>
-      <c r="AC38" s="0" t="s">
+      <c r="AC38" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>269</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>240</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="3">
         <v>30</v>
       </c>
-      <c r="D39" s="4" t="n">
+      <c r="D39" s="4">
         <v>5</v>
       </c>
-      <c r="E39" s="4" t="n">
+      <c r="E39" s="4">
         <v>2</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="G39" t="s">
         <v>270</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="H39" t="s">
         <v>271</v>
       </c>
-      <c r="J39" s="0" t="s">
+      <c r="J39" t="s">
         <v>270</v>
       </c>
-      <c r="K39" s="0" t="s">
+      <c r="K39" t="s">
         <v>271</v>
       </c>
-      <c r="M39" s="0" t="s">
+      <c r="M39" t="s">
         <v>270</v>
       </c>
-      <c r="N39" s="0" t="s">
+      <c r="N39" t="s">
         <v>271</v>
       </c>
-      <c r="P39" s="0" t="s">
+      <c r="P39" t="s">
         <v>272</v>
       </c>
-      <c r="Q39" s="0" t="s">
+      <c r="Q39" t="s">
         <v>273</v>
       </c>
-      <c r="S39" s="0" t="s">
+      <c r="S39" t="s">
         <v>270</v>
       </c>
-      <c r="T39" s="0" t="s">
+      <c r="T39" t="s">
         <v>271</v>
       </c>
-      <c r="V39" s="0" t="s">
+      <c r="V39" t="s">
         <v>274</v>
       </c>
-      <c r="W39" s="0" t="s">
+      <c r="W39" t="s">
         <v>275</v>
       </c>
-      <c r="Y39" s="0" t="s">
+      <c r="Y39" t="s">
         <v>270</v>
       </c>
-      <c r="Z39" s="0" t="s">
+      <c r="Z39" t="s">
         <v>271</v>
       </c>
-      <c r="AB39" s="0" t="s">
+      <c r="AB39" t="s">
         <v>270</v>
       </c>
-      <c r="AC39" s="0" t="s">
+      <c r="AC39" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>240</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="3">
         <v>12</v>
       </c>
-      <c r="D40" s="4" t="n">
+      <c r="D40" s="4">
         <v>8</v>
       </c>
-      <c r="E40" s="4" t="n">
+      <c r="E40" s="4">
         <v>1</v>
       </c>
-      <c r="G40" s="0" t="s">
+      <c r="G40" t="s">
         <v>277</v>
       </c>
-      <c r="H40" s="0" t="s">
+      <c r="H40" t="s">
         <v>278</v>
       </c>
-      <c r="J40" s="0" t="s">
+      <c r="J40" t="s">
         <v>277</v>
       </c>
-      <c r="K40" s="0" t="s">
+      <c r="K40" t="s">
         <v>278</v>
       </c>
-      <c r="M40" s="0" t="s">
+      <c r="M40" t="s">
         <v>277</v>
       </c>
-      <c r="N40" s="0" t="s">
+      <c r="N40" t="s">
         <v>278</v>
       </c>
-      <c r="P40" s="0" t="s">
+      <c r="P40" t="s">
         <v>279</v>
       </c>
-      <c r="Q40" s="0" t="s">
+      <c r="Q40" t="s">
         <v>280</v>
       </c>
-      <c r="S40" s="0" t="s">
+      <c r="S40" t="s">
         <v>277</v>
       </c>
-      <c r="T40" s="0" t="s">
+      <c r="T40" t="s">
         <v>278</v>
       </c>
-      <c r="V40" s="0" t="s">
+      <c r="V40" t="s">
         <v>281</v>
       </c>
-      <c r="W40" s="0" t="s">
+      <c r="W40" t="s">
         <v>282</v>
       </c>
-      <c r="Y40" s="0" t="s">
+      <c r="Y40" t="s">
         <v>277</v>
       </c>
-      <c r="Z40" s="0" t="s">
+      <c r="Z40" t="s">
         <v>278</v>
       </c>
-      <c r="AB40" s="0" t="s">
+      <c r="AB40" t="s">
         <v>277</v>
       </c>
-      <c r="AC40" s="0" t="s">
+      <c r="AC40" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>283</v>
       </c>
-      <c r="C42" s="4" t="n">
+      <c r="C42" s="4">
         <v>1916</v>
       </c>
-      <c r="D42" s="4" t="n">
+      <c r="D42" s="4">
         <v>546</v>
       </c>
-      <c r="E42" s="4" t="n">
+      <c r="E42" s="4">
         <v>51</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>284</v>
       </c>
-      <c r="C43" s="4" t="n">
+      <c r="C43" s="4">
         <v>3832</v>
       </c>
-      <c r="D43" s="4" t="n">
+      <c r="D43" s="4">
         <v>1092</v>
       </c>
-      <c r="E43" s="4" t="n">
+      <c r="E43" s="4">
         <v>153</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
         <v>285</v>
       </c>
-      <c r="C44" s="4" t="n">
+      <c r="C44" s="4">
         <v>3832</v>
       </c>
-      <c r="D44" s="4" t="n">
+      <c r="D44" s="4">
         <v>1245</v>
       </c>
-      <c r="E44" s="4" t="n">
+      <c r="E44" s="4">
         <v>1245</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H2:H40 A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCellId="1" sqref="H2:H40 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.77734375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H2:H40 A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCellId="1" sqref="H2:H40 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.77734375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some more code related to the level pointer table
</commit_message>
<xml_diff>
--- a/SMB1/Research Docs/Level Offsets.xlsx
+++ b/SMB1/Research Docs/Level Offsets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="864"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8136" tabRatio="864"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1225,7 +1225,9 @@
   </sheetPr>
   <dimension ref="A1:AD44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3952,7 +3954,7 @@
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+      <c r="A42" t="s">
         <v>283</v>
       </c>
       <c r="C42" s="4">
@@ -3966,7 +3968,7 @@
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+      <c r="A43" t="s">
         <v>284</v>
       </c>
       <c r="C43" s="4">
@@ -3980,7 +3982,7 @@
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
+      <c r="A44" t="s">
         <v>285</v>
       </c>
       <c r="C44" s="4">

</xml_diff>

<commit_message>
Pipe pointers now properly ignore the page flag. Support for the page flag with pipe pointers will be added once the feature freeze ends.
</commit_message>
<xml_diff>
--- a/SMB1/Research Docs/Level Offsets.xlsx
+++ b/SMB1/Research Docs/Level Offsets.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="920" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="920"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -979,33 +978,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1017,7 +997,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1025,3024 +1005,3256 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AE44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.219387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.219387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3316326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.219387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.77551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1020408163265"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.219387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.77551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.8877551020408"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0051020408163"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.55612244897959"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.1071428571429"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.8928571428571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.6632653061224"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.8877551020408"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.77551020408163"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.4438775510204"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="21.5561224489796"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.8928571428571"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.4438775510204"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.10714285714286"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="21.6632653061224"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="21.780612244898"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="7.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="11.7704081632653"/>
+    <col min="1" max="1" width="20.21875"/>
+    <col min="2" max="2" width="11.44140625"/>
+    <col min="3" max="3" width="14.109375"/>
+    <col min="4" max="4" width="11.5546875"/>
+    <col min="5" max="5" width="12.21875"/>
+    <col min="6" max="6" width="16"/>
+    <col min="7" max="7" width="10.33203125"/>
+    <col min="8" max="8" width="21.109375"/>
+    <col min="9" max="9" width="21.21875"/>
+    <col min="10" max="10" width="7.77734375"/>
+    <col min="11" max="11" width="21.109375"/>
+    <col min="12" max="12" width="21.21875"/>
+    <col min="13" max="13" width="7.77734375"/>
+    <col min="14" max="14" width="22.88671875"/>
+    <col min="15" max="15" width="23"/>
+    <col min="16" max="16" width="8.5546875"/>
+    <col min="17" max="17" width="19"/>
+    <col min="18" max="18" width="19.109375"/>
+    <col min="19" max="19" width="16.88671875"/>
+    <col min="20" max="20" width="20.6640625"/>
+    <col min="21" max="21" width="20.88671875"/>
+    <col min="22" max="22" width="7.77734375"/>
+    <col min="23" max="23" width="21.44140625"/>
+    <col min="24" max="24" width="21.5546875"/>
+    <col min="25" max="25" width="16.88671875"/>
+    <col min="26" max="26" width="22.44140625"/>
+    <col min="27" max="27" width="22.5546875"/>
+    <col min="28" max="28" width="8.109375"/>
+    <col min="29" max="29" width="21.6640625"/>
+    <col min="30" max="30" width="21.77734375"/>
+    <col min="31" max="31" width="7.77734375"/>
+    <col min="32" max="1025" width="11.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="3">
         <v>49</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="3">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="3">
         <v>1</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="0" t="s">
+      <c r="H2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="S2" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" t="s">
         <v>34</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="U2" t="s">
         <v>35</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="V2" t="s">
         <v>36</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" t="s">
         <v>40</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="X2" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Y2" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AA2" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AB2" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AC2" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AD2" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AE2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="3">
         <v>80</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="3">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="3">
         <v>2</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="0" t="s">
+      <c r="H3" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="U3" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="X3" t="s">
         <v>50</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" t="s">
         <v>51</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AA3" t="s">
         <v>45</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="AC3" t="s">
         <v>44</v>
       </c>
-      <c r="AD3" s="0" t="s">
+      <c r="AD3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="3">
         <v>41</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="3">
         <v>14</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="0" t="s">
+      <c r="H4" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="L4" t="s">
         <v>56</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" t="s">
         <v>55</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" t="s">
         <v>56</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="R4" t="s">
         <v>58</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="T4" t="s">
         <v>55</v>
       </c>
-      <c r="U4" s="0" t="s">
+      <c r="U4" t="s">
         <v>56</v>
       </c>
-      <c r="W4" s="0" t="s">
+      <c r="W4" t="s">
         <v>59</v>
       </c>
-      <c r="X4" s="0" t="s">
+      <c r="X4" t="s">
         <v>60</v>
       </c>
-      <c r="Z4" s="0" t="s">
+      <c r="Z4" t="s">
         <v>55</v>
       </c>
-      <c r="AA4" s="0" t="s">
+      <c r="AA4" t="s">
         <v>56</v>
       </c>
-      <c r="AC4" s="0" t="s">
+      <c r="AC4" t="s">
         <v>55</v>
       </c>
-      <c r="AD4" s="0" t="s">
+      <c r="AD4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="3">
         <v>47</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="3">
         <v>19</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="3">
         <v>0</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="0" t="s">
+      <c r="H5" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="L5" t="s">
         <v>65</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="N5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="O5" t="s">
         <v>65</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" t="s">
         <v>66</v>
       </c>
-      <c r="R5" s="0" t="s">
+      <c r="R5" t="s">
         <v>67</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="T5" t="s">
         <v>64</v>
       </c>
-      <c r="U5" s="0" t="s">
+      <c r="U5" t="s">
         <v>65</v>
       </c>
-      <c r="W5" s="0" t="s">
+      <c r="W5" t="s">
         <v>68</v>
       </c>
-      <c r="X5" s="0" t="s">
+      <c r="X5" t="s">
         <v>69</v>
       </c>
-      <c r="Z5" s="0" t="s">
+      <c r="Z5" t="s">
         <v>64</v>
       </c>
-      <c r="AA5" s="0" t="s">
+      <c r="AA5" t="s">
         <v>65</v>
       </c>
-      <c r="AC5" s="0" t="s">
+      <c r="AC5" t="s">
         <v>64</v>
       </c>
-      <c r="AD5" s="0" t="s">
+      <c r="AD5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="3">
         <v>49</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="3">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="3">
         <v>2</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="0" t="s">
+      <c r="H6" t="s">
         <v>72</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>73</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="L6" t="s">
         <v>73</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="N6" t="s">
         <v>72</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="O6" t="s">
         <v>73</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" t="s">
         <v>74</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="R6" t="s">
         <v>75</v>
       </c>
-      <c r="T6" s="0" t="s">
+      <c r="T6" t="s">
         <v>72</v>
       </c>
-      <c r="U6" s="0" t="s">
+      <c r="U6" t="s">
         <v>73</v>
       </c>
-      <c r="W6" s="0" t="s">
+      <c r="W6" t="s">
         <v>76</v>
       </c>
-      <c r="X6" s="0" t="s">
+      <c r="X6" t="s">
         <v>77</v>
       </c>
-      <c r="Z6" s="0" t="s">
+      <c r="Z6" t="s">
         <v>72</v>
       </c>
-      <c r="AA6" s="0" t="s">
+      <c r="AA6" t="s">
         <v>73</v>
       </c>
-      <c r="AC6" s="0" t="s">
+      <c r="AC6" t="s">
         <v>72</v>
       </c>
-      <c r="AD6" s="0" t="s">
+      <c r="AD6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="3">
         <v>60</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="3">
         <v>16</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="3">
         <v>3</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="0" t="s">
+      <c r="H7" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>82</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" t="s">
         <v>81</v>
       </c>
-      <c r="L7" s="0" t="s">
+      <c r="L7" t="s">
         <v>82</v>
       </c>
-      <c r="N7" s="0" t="s">
+      <c r="N7" t="s">
         <v>81</v>
       </c>
-      <c r="O7" s="0" t="s">
+      <c r="O7" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" t="s">
         <v>83</v>
       </c>
-      <c r="R7" s="0" t="s">
+      <c r="R7" t="s">
         <v>84</v>
       </c>
-      <c r="T7" s="0" t="s">
+      <c r="T7" t="s">
         <v>81</v>
       </c>
-      <c r="U7" s="0" t="s">
+      <c r="U7" t="s">
         <v>82</v>
       </c>
-      <c r="W7" s="0" t="s">
+      <c r="W7" t="s">
         <v>85</v>
       </c>
-      <c r="X7" s="0" t="s">
+      <c r="X7" t="s">
         <v>86</v>
       </c>
-      <c r="Z7" s="0" t="s">
+      <c r="Z7" t="s">
         <v>81</v>
       </c>
-      <c r="AA7" s="0" t="s">
+      <c r="AA7" t="s">
         <v>82</v>
       </c>
-      <c r="AC7" s="0" t="s">
+      <c r="AC7" t="s">
         <v>81</v>
       </c>
-      <c r="AD7" s="0" t="s">
+      <c r="AD7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="3">
         <v>65</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="3">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="3">
         <v>0</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="0" t="s">
+      <c r="H8" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" t="s">
         <v>90</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="L8" t="s">
         <v>91</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="N8" t="s">
         <v>90</v>
       </c>
-      <c r="O8" s="0" t="s">
+      <c r="O8" t="s">
         <v>91</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" t="s">
         <v>92</v>
       </c>
-      <c r="R8" s="0" t="s">
+      <c r="R8" t="s">
         <v>93</v>
       </c>
-      <c r="T8" s="0" t="s">
+      <c r="T8" t="s">
         <v>90</v>
       </c>
-      <c r="U8" s="0" t="s">
+      <c r="U8" t="s">
         <v>91</v>
       </c>
-      <c r="W8" s="0" t="s">
+      <c r="W8" t="s">
         <v>94</v>
       </c>
-      <c r="X8" s="0" t="s">
+      <c r="X8" t="s">
         <v>95</v>
       </c>
-      <c r="Z8" s="0" t="s">
+      <c r="Z8" t="s">
         <v>90</v>
       </c>
-      <c r="AA8" s="0" t="s">
+      <c r="AA8" t="s">
         <v>91</v>
       </c>
-      <c r="AC8" s="0" t="s">
+      <c r="AC8" t="s">
         <v>90</v>
       </c>
-      <c r="AD8" s="0" t="s">
+      <c r="AD8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="3">
         <v>56</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="3">
         <v>23</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="3">
         <v>0</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="0" t="s">
+      <c r="H9" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" t="s">
         <v>100</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" t="s">
         <v>99</v>
       </c>
-      <c r="L9" s="0" t="s">
+      <c r="L9" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="0" t="s">
+      <c r="N9" t="s">
         <v>99</v>
       </c>
-      <c r="O9" s="0" t="s">
+      <c r="O9" t="s">
         <v>100</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" t="s">
         <v>101</v>
       </c>
-      <c r="R9" s="0" t="s">
+      <c r="R9" t="s">
         <v>102</v>
       </c>
-      <c r="T9" s="0" t="s">
+      <c r="T9" t="s">
         <v>99</v>
       </c>
-      <c r="U9" s="0" t="s">
+      <c r="U9" t="s">
         <v>100</v>
       </c>
-      <c r="W9" s="0" t="s">
+      <c r="W9" t="s">
         <v>103</v>
       </c>
-      <c r="X9" s="0" t="s">
+      <c r="X9" t="s">
         <v>104</v>
       </c>
-      <c r="Z9" s="0" t="s">
+      <c r="Z9" t="s">
         <v>99</v>
       </c>
-      <c r="AA9" s="0" t="s">
+      <c r="AA9" t="s">
         <v>100</v>
       </c>
-      <c r="AC9" s="0" t="s">
+      <c r="AC9" t="s">
         <v>99</v>
       </c>
-      <c r="AD9" s="0" t="s">
+      <c r="AD9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="3">
         <v>57</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="3">
         <v>21</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="3">
         <v>2</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="0" t="s">
+      <c r="H10" t="s">
         <v>107</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" t="s">
         <v>108</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" t="s">
         <v>107</v>
       </c>
-      <c r="L10" s="0" t="s">
+      <c r="L10" t="s">
         <v>108</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="N10" t="s">
         <v>107</v>
       </c>
-      <c r="O10" s="0" t="s">
+      <c r="O10" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" t="s">
         <v>109</v>
       </c>
-      <c r="R10" s="0" t="s">
+      <c r="R10" t="s">
         <v>110</v>
       </c>
-      <c r="T10" s="0" t="s">
+      <c r="T10" t="s">
         <v>107</v>
       </c>
-      <c r="U10" s="0" t="s">
+      <c r="U10" t="s">
         <v>108</v>
       </c>
-      <c r="W10" s="0" t="s">
+      <c r="W10" t="s">
         <v>111</v>
       </c>
-      <c r="X10" s="0" t="s">
+      <c r="X10" t="s">
         <v>112</v>
       </c>
-      <c r="Z10" s="0" t="s">
+      <c r="Z10" t="s">
         <v>107</v>
       </c>
-      <c r="AA10" s="0" t="s">
+      <c r="AA10" t="s">
         <v>108</v>
       </c>
-      <c r="AC10" s="0" t="s">
+      <c r="AC10" t="s">
         <v>107</v>
       </c>
-      <c r="AD10" s="0" t="s">
+      <c r="AD10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="3">
         <v>24</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="3">
         <v>18</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="3">
         <v>0</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="0" t="s">
+      <c r="H11" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" t="s">
         <v>115</v>
       </c>
-      <c r="L11" s="0" t="s">
+      <c r="L11" t="s">
         <v>116</v>
       </c>
-      <c r="N11" s="0" t="s">
+      <c r="N11" t="s">
         <v>115</v>
       </c>
-      <c r="O11" s="0" t="s">
+      <c r="O11" t="s">
         <v>116</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" t="s">
         <v>117</v>
       </c>
-      <c r="R11" s="0" t="s">
+      <c r="R11" t="s">
         <v>118</v>
       </c>
-      <c r="T11" s="0" t="s">
+      <c r="T11" t="s">
         <v>115</v>
       </c>
-      <c r="U11" s="0" t="s">
+      <c r="U11" t="s">
         <v>116</v>
       </c>
-      <c r="W11" s="0" t="s">
+      <c r="W11" t="s">
         <v>119</v>
       </c>
-      <c r="X11" s="0" t="s">
+      <c r="X11" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="0" t="s">
+      <c r="Z11" t="s">
         <v>115</v>
       </c>
-      <c r="AA11" s="0" t="s">
+      <c r="AA11" t="s">
         <v>116</v>
       </c>
-      <c r="AC11" s="0" t="s">
+      <c r="AC11" t="s">
         <v>115</v>
       </c>
-      <c r="AD11" s="0" t="s">
+      <c r="AD11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="3">
         <v>48</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="3">
         <v>18</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="3">
         <v>0</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="0" t="s">
+      <c r="H12" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="K12" t="s">
         <v>123</v>
       </c>
-      <c r="L12" s="0" t="s">
+      <c r="L12" t="s">
         <v>124</v>
       </c>
-      <c r="N12" s="0" t="s">
+      <c r="N12" t="s">
         <v>123</v>
       </c>
-      <c r="O12" s="0" t="s">
+      <c r="O12" t="s">
         <v>124</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" t="s">
         <v>125</v>
       </c>
-      <c r="R12" s="0" t="s">
+      <c r="R12" t="s">
         <v>126</v>
       </c>
-      <c r="T12" s="0" t="s">
+      <c r="T12" t="s">
         <v>123</v>
       </c>
-      <c r="U12" s="0" t="s">
+      <c r="U12" t="s">
         <v>124</v>
       </c>
-      <c r="W12" s="0" t="s">
+      <c r="W12" t="s">
         <v>127</v>
       </c>
-      <c r="X12" s="0" t="s">
+      <c r="X12" t="s">
         <v>128</v>
       </c>
-      <c r="Z12" s="0" t="s">
+      <c r="Z12" t="s">
         <v>123</v>
       </c>
-      <c r="AA12" s="0" t="s">
+      <c r="AA12" t="s">
         <v>124</v>
       </c>
-      <c r="AC12" s="0" t="s">
+      <c r="AC12" t="s">
         <v>123</v>
       </c>
-      <c r="AD12" s="0" t="s">
+      <c r="AD12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="3">
         <v>53</v>
       </c>
-      <c r="E13" s="3" t="n">
+      <c r="E13" s="3">
         <v>21</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="3">
         <v>0</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="0" t="s">
+      <c r="H13" t="s">
         <v>131</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" t="s">
         <v>132</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="K13" t="s">
         <v>131</v>
       </c>
-      <c r="L13" s="0" t="s">
+      <c r="L13" t="s">
         <v>132</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="N13" t="s">
         <v>131</v>
       </c>
-      <c r="O13" s="0" t="s">
+      <c r="O13" t="s">
         <v>132</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" t="s">
         <v>133</v>
       </c>
-      <c r="R13" s="0" t="s">
+      <c r="R13" t="s">
         <v>134</v>
       </c>
-      <c r="T13" s="0" t="s">
+      <c r="T13" t="s">
         <v>131</v>
       </c>
-      <c r="U13" s="0" t="s">
+      <c r="U13" t="s">
         <v>132</v>
       </c>
-      <c r="W13" s="0" t="s">
+      <c r="W13" t="s">
         <v>135</v>
       </c>
-      <c r="X13" s="0" t="s">
+      <c r="X13" t="s">
         <v>136</v>
       </c>
-      <c r="Z13" s="0" t="s">
+      <c r="Z13" t="s">
         <v>131</v>
       </c>
-      <c r="AA13" s="0" t="s">
+      <c r="AA13" t="s">
         <v>132</v>
       </c>
-      <c r="AC13" s="0" t="s">
+      <c r="AC13" t="s">
         <v>131</v>
       </c>
-      <c r="AD13" s="0" t="s">
+      <c r="AD13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="3">
         <v>40</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="3">
         <v>5</v>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="3">
         <v>1</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="0" t="s">
+      <c r="H14" t="s">
         <v>139</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" t="s">
         <v>140</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" t="s">
         <v>139</v>
       </c>
-      <c r="L14" s="0" t="s">
+      <c r="L14" t="s">
         <v>140</v>
       </c>
-      <c r="N14" s="0" t="s">
+      <c r="N14" t="s">
         <v>139</v>
       </c>
-      <c r="O14" s="0" t="s">
+      <c r="O14" t="s">
         <v>140</v>
       </c>
-      <c r="Q14" s="0" t="s">
+      <c r="Q14" t="s">
         <v>141</v>
       </c>
-      <c r="R14" s="0" t="s">
+      <c r="R14" t="s">
         <v>142</v>
       </c>
-      <c r="T14" s="0" t="s">
+      <c r="T14" t="s">
         <v>139</v>
       </c>
-      <c r="U14" s="0" t="s">
+      <c r="U14" t="s">
         <v>140</v>
       </c>
-      <c r="W14" s="0" t="s">
+      <c r="W14" t="s">
         <v>143</v>
       </c>
-      <c r="X14" s="0" t="s">
+      <c r="X14" t="s">
         <v>144</v>
       </c>
-      <c r="Z14" s="0" t="s">
+      <c r="Z14" t="s">
         <v>139</v>
       </c>
-      <c r="AA14" s="0" t="s">
+      <c r="AA14" t="s">
         <v>140</v>
       </c>
-      <c r="AC14" s="0" t="s">
+      <c r="AC14" t="s">
         <v>139</v>
       </c>
-      <c r="AD14" s="0" t="s">
+      <c r="AD14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>146</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="3">
         <v>79</v>
       </c>
-      <c r="E15" s="3" t="n">
+      <c r="E15" s="3">
         <v>18</v>
       </c>
-      <c r="F15" s="3" t="n">
+      <c r="F15" s="3">
         <v>3</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="0" t="s">
+      <c r="H15" t="s">
         <v>147</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" t="s">
         <v>148</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K15" t="s">
         <v>147</v>
       </c>
-      <c r="L15" s="0" t="s">
+      <c r="L15" t="s">
         <v>148</v>
       </c>
-      <c r="N15" s="0" t="s">
+      <c r="N15" t="s">
         <v>147</v>
       </c>
-      <c r="O15" s="0" t="s">
+      <c r="O15" t="s">
         <v>148</v>
       </c>
-      <c r="Q15" s="0" t="s">
+      <c r="Q15" t="s">
         <v>149</v>
       </c>
-      <c r="R15" s="0" t="s">
+      <c r="R15" t="s">
         <v>150</v>
       </c>
-      <c r="T15" s="0" t="s">
+      <c r="T15" t="s">
         <v>147</v>
       </c>
-      <c r="U15" s="0" t="s">
+      <c r="U15" t="s">
         <v>148</v>
       </c>
-      <c r="W15" s="0" t="s">
+      <c r="W15" t="s">
         <v>151</v>
       </c>
-      <c r="X15" s="0" t="s">
+      <c r="X15" t="s">
         <v>152</v>
       </c>
-      <c r="Z15" s="0" t="s">
+      <c r="Z15" t="s">
         <v>147</v>
       </c>
-      <c r="AA15" s="0" t="s">
+      <c r="AA15" t="s">
         <v>148</v>
       </c>
-      <c r="AC15" s="0" t="s">
+      <c r="AC15" t="s">
         <v>147</v>
       </c>
-      <c r="AD15" s="0" t="s">
+      <c r="AD15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>154</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="3">
         <v>50</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E16" s="3">
         <v>18</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="3">
         <v>0</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="0" t="s">
+      <c r="H16" t="s">
         <v>155</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" t="s">
         <v>156</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" t="s">
         <v>155</v>
       </c>
-      <c r="L16" s="0" t="s">
+      <c r="L16" t="s">
         <v>156</v>
       </c>
-      <c r="N16" s="0" t="s">
+      <c r="N16" t="s">
         <v>155</v>
       </c>
-      <c r="O16" s="0" t="s">
+      <c r="O16" t="s">
         <v>156</v>
       </c>
-      <c r="Q16" s="0" t="s">
+      <c r="Q16" t="s">
         <v>157</v>
       </c>
-      <c r="R16" s="0" t="s">
+      <c r="R16" t="s">
         <v>158</v>
       </c>
-      <c r="T16" s="0" t="s">
+      <c r="T16" t="s">
         <v>155</v>
       </c>
-      <c r="U16" s="0" t="s">
+      <c r="U16" t="s">
         <v>156</v>
       </c>
-      <c r="W16" s="0" t="s">
+      <c r="W16" t="s">
         <v>159</v>
       </c>
-      <c r="X16" s="0" t="s">
+      <c r="X16" t="s">
         <v>160</v>
       </c>
-      <c r="Z16" s="0" t="s">
+      <c r="Z16" t="s">
         <v>155</v>
       </c>
-      <c r="AA16" s="0" t="s">
+      <c r="AA16" t="s">
         <v>156</v>
       </c>
-      <c r="AC16" s="0" t="s">
+      <c r="AC16" t="s">
         <v>155</v>
       </c>
-      <c r="AD16" s="0" t="s">
+      <c r="AD16" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>162</v>
       </c>
-      <c r="D17" s="3" t="n">
+      <c r="D17" s="3">
         <v>62</v>
       </c>
-      <c r="E17" s="3" t="n">
+      <c r="E17" s="3">
         <v>12</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" s="3">
         <v>0</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="0" t="s">
+      <c r="H17" t="s">
         <v>163</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" t="s">
         <v>164</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="K17" t="s">
         <v>163</v>
       </c>
-      <c r="L17" s="0" t="s">
+      <c r="L17" t="s">
         <v>164</v>
       </c>
-      <c r="N17" s="0" t="s">
+      <c r="N17" t="s">
         <v>163</v>
       </c>
-      <c r="O17" s="0" t="s">
+      <c r="O17" t="s">
         <v>164</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q17" t="s">
         <v>165</v>
       </c>
-      <c r="R17" s="0" t="s">
+      <c r="R17" t="s">
         <v>166</v>
       </c>
-      <c r="T17" s="0" t="s">
+      <c r="T17" t="s">
         <v>163</v>
       </c>
-      <c r="U17" s="0" t="s">
+      <c r="U17" t="s">
         <v>164</v>
       </c>
-      <c r="W17" s="0" t="s">
+      <c r="W17" t="s">
         <v>167</v>
       </c>
-      <c r="X17" s="0" t="s">
+      <c r="X17" t="s">
         <v>168</v>
       </c>
-      <c r="Z17" s="0" t="s">
+      <c r="Z17" t="s">
         <v>163</v>
       </c>
-      <c r="AA17" s="0" t="s">
+      <c r="AA17" t="s">
         <v>164</v>
       </c>
-      <c r="AC17" s="0" t="s">
+      <c r="AC17" t="s">
         <v>163</v>
       </c>
-      <c r="AD17" s="0" t="s">
+      <c r="AD17" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>170</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="3">
         <v>30</v>
       </c>
-      <c r="E18" s="3" t="n">
+      <c r="E18" s="3">
         <v>16</v>
       </c>
-      <c r="F18" s="3" t="n">
+      <c r="F18" s="3">
         <v>1</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="0" t="s">
+      <c r="H18" t="s">
         <v>171</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" t="s">
         <v>172</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="K18" t="s">
         <v>171</v>
       </c>
-      <c r="L18" s="0" t="s">
+      <c r="L18" t="s">
         <v>172</v>
       </c>
-      <c r="N18" s="0" t="s">
+      <c r="N18" t="s">
         <v>171</v>
       </c>
-      <c r="O18" s="0" t="s">
+      <c r="O18" t="s">
         <v>172</v>
       </c>
-      <c r="Q18" s="0" t="s">
+      <c r="Q18" t="s">
         <v>173</v>
       </c>
-      <c r="R18" s="0" t="s">
+      <c r="R18" t="s">
         <v>174</v>
       </c>
-      <c r="T18" s="0" t="s">
+      <c r="T18" t="s">
         <v>171</v>
       </c>
-      <c r="U18" s="0" t="s">
+      <c r="U18" t="s">
         <v>172</v>
       </c>
-      <c r="W18" s="0" t="s">
+      <c r="W18" t="s">
         <v>175</v>
       </c>
-      <c r="X18" s="0" t="s">
+      <c r="X18" t="s">
         <v>176</v>
       </c>
-      <c r="Z18" s="0" t="s">
+      <c r="Z18" t="s">
         <v>171</v>
       </c>
-      <c r="AA18" s="0" t="s">
+      <c r="AA18" t="s">
         <v>172</v>
       </c>
-      <c r="AC18" s="0" t="s">
+      <c r="AC18" t="s">
         <v>171</v>
       </c>
-      <c r="AD18" s="0" t="s">
+      <c r="AD18" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>178</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="3">
         <v>56</v>
       </c>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="3">
         <v>18</v>
       </c>
-      <c r="F19" s="3" t="n">
+      <c r="F19" s="3">
         <v>2</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="0" t="s">
+      <c r="H19" t="s">
         <v>179</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" t="s">
         <v>180</v>
       </c>
-      <c r="K19" s="0" t="s">
+      <c r="K19" t="s">
         <v>179</v>
       </c>
-      <c r="L19" s="0" t="s">
+      <c r="L19" t="s">
         <v>180</v>
       </c>
-      <c r="N19" s="0" t="s">
+      <c r="N19" t="s">
         <v>179</v>
       </c>
-      <c r="O19" s="0" t="s">
+      <c r="O19" t="s">
         <v>180</v>
       </c>
-      <c r="Q19" s="0" t="s">
+      <c r="Q19" t="s">
         <v>181</v>
       </c>
-      <c r="R19" s="0" t="s">
+      <c r="R19" t="s">
         <v>182</v>
       </c>
-      <c r="T19" s="0" t="s">
+      <c r="T19" t="s">
         <v>179</v>
       </c>
-      <c r="U19" s="0" t="s">
+      <c r="U19" t="s">
         <v>180</v>
       </c>
-      <c r="W19" s="0" t="s">
+      <c r="W19" t="s">
         <v>183</v>
       </c>
-      <c r="X19" s="0" t="s">
+      <c r="X19" t="s">
         <v>184</v>
       </c>
-      <c r="Z19" s="0" t="s">
+      <c r="Z19" t="s">
         <v>179</v>
       </c>
-      <c r="AA19" s="0" t="s">
+      <c r="AA19" t="s">
         <v>180</v>
       </c>
-      <c r="AC19" s="0" t="s">
+      <c r="AC19" t="s">
         <v>179</v>
       </c>
-      <c r="AD19" s="0" t="s">
+      <c r="AD19" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>187</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="3">
         <v>41</v>
       </c>
-      <c r="E20" s="3" t="n">
+      <c r="E20" s="3">
         <v>14</v>
       </c>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="3">
         <v>0</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="0" t="s">
+      <c r="H20" t="s">
         <v>55</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" t="s">
         <v>55</v>
       </c>
-      <c r="L20" s="0" t="s">
+      <c r="L20" t="s">
         <v>56</v>
       </c>
-      <c r="N20" s="0" t="s">
+      <c r="N20" t="s">
         <v>55</v>
       </c>
-      <c r="O20" s="0" t="s">
+      <c r="O20" t="s">
         <v>56</v>
       </c>
-      <c r="Q20" s="0" t="s">
+      <c r="Q20" t="s">
         <v>57</v>
       </c>
-      <c r="R20" s="0" t="s">
+      <c r="R20" t="s">
         <v>58</v>
       </c>
-      <c r="T20" s="0" t="s">
+      <c r="T20" t="s">
         <v>55</v>
       </c>
-      <c r="U20" s="0" t="s">
+      <c r="U20" t="s">
         <v>56</v>
       </c>
-      <c r="W20" s="0" t="s">
+      <c r="W20" t="s">
         <v>59</v>
       </c>
-      <c r="X20" s="0" t="s">
+      <c r="X20" t="s">
         <v>60</v>
       </c>
-      <c r="Z20" s="0" t="s">
+      <c r="Z20" t="s">
         <v>55</v>
       </c>
-      <c r="AA20" s="0" t="s">
+      <c r="AA20" t="s">
         <v>56</v>
       </c>
-      <c r="AC20" s="0" t="s">
+      <c r="AC20" t="s">
         <v>55</v>
       </c>
-      <c r="AD20" s="0" t="s">
+      <c r="AD20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>189</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>190</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="3">
         <v>56</v>
       </c>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="3">
         <v>23</v>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="3">
         <v>0</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="0" t="s">
+      <c r="H21" t="s">
         <v>99</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" t="s">
         <v>100</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="K21" t="s">
         <v>99</v>
       </c>
-      <c r="L21" s="0" t="s">
+      <c r="L21" t="s">
         <v>100</v>
       </c>
-      <c r="N21" s="0" t="s">
+      <c r="N21" t="s">
         <v>99</v>
       </c>
-      <c r="O21" s="0" t="s">
+      <c r="O21" t="s">
         <v>100</v>
       </c>
-      <c r="Q21" s="0" t="s">
+      <c r="Q21" t="s">
         <v>101</v>
       </c>
-      <c r="R21" s="0" t="s">
+      <c r="R21" t="s">
         <v>102</v>
       </c>
-      <c r="T21" s="0" t="s">
+      <c r="T21" t="s">
         <v>99</v>
       </c>
-      <c r="U21" s="0" t="s">
+      <c r="U21" t="s">
         <v>100</v>
       </c>
-      <c r="W21" s="0" t="s">
+      <c r="W21" t="s">
         <v>103</v>
       </c>
-      <c r="X21" s="0" t="s">
+      <c r="X21" t="s">
         <v>104</v>
       </c>
-      <c r="Z21" s="0" t="s">
+      <c r="Z21" t="s">
         <v>99</v>
       </c>
-      <c r="AA21" s="0" t="s">
+      <c r="AA21" t="s">
         <v>100</v>
       </c>
-      <c r="AC21" s="0" t="s">
+      <c r="AC21" t="s">
         <v>99</v>
       </c>
-      <c r="AD21" s="0" t="s">
+      <c r="AD21" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>192</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="3">
         <v>56</v>
       </c>
-      <c r="E22" s="3" t="n">
+      <c r="E22" s="3">
         <v>4</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="3">
         <v>0</v>
       </c>
       <c r="G22" s="3"/>
-      <c r="H22" s="0" t="s">
+      <c r="H22" t="s">
         <v>193</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" t="s">
         <v>194</v>
       </c>
-      <c r="K22" s="0" t="s">
+      <c r="K22" t="s">
         <v>193</v>
       </c>
-      <c r="L22" s="0" t="s">
+      <c r="L22" t="s">
         <v>194</v>
       </c>
-      <c r="N22" s="0" t="s">
+      <c r="N22" t="s">
         <v>193</v>
       </c>
-      <c r="O22" s="0" t="s">
+      <c r="O22" t="s">
         <v>194</v>
       </c>
-      <c r="Q22" s="0" t="s">
+      <c r="Q22" t="s">
         <v>195</v>
       </c>
-      <c r="R22" s="0" t="s">
+      <c r="R22" t="s">
         <v>196</v>
       </c>
-      <c r="T22" s="0" t="s">
+      <c r="T22" t="s">
         <v>193</v>
       </c>
-      <c r="U22" s="0" t="s">
+      <c r="U22" t="s">
         <v>194</v>
       </c>
-      <c r="W22" s="0" t="s">
+      <c r="W22" t="s">
         <v>197</v>
       </c>
-      <c r="X22" s="0" t="s">
+      <c r="X22" t="s">
         <v>198</v>
       </c>
-      <c r="Z22" s="0" t="s">
+      <c r="Z22" t="s">
         <v>193</v>
       </c>
-      <c r="AA22" s="0" t="s">
+      <c r="AA22" t="s">
         <v>194</v>
       </c>
-      <c r="AC22" s="0" t="s">
+      <c r="AC22" t="s">
         <v>193</v>
       </c>
-      <c r="AD22" s="0" t="s">
+      <c r="AD22" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>200</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="3">
         <v>70</v>
       </c>
-      <c r="E23" s="3" t="n">
+      <c r="E23" s="3">
         <v>13</v>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="3">
         <v>4</v>
       </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="0" t="s">
+      <c r="H23" t="s">
         <v>201</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" t="s">
         <v>202</v>
       </c>
-      <c r="K23" s="0" t="s">
+      <c r="K23" t="s">
         <v>201</v>
       </c>
-      <c r="L23" s="0" t="s">
+      <c r="L23" t="s">
         <v>202</v>
       </c>
-      <c r="N23" s="0" t="s">
+      <c r="N23" t="s">
         <v>201</v>
       </c>
-      <c r="O23" s="0" t="s">
+      <c r="O23" t="s">
         <v>202</v>
       </c>
-      <c r="Q23" s="0" t="s">
+      <c r="Q23" t="s">
         <v>203</v>
       </c>
-      <c r="R23" s="0" t="s">
+      <c r="R23" t="s">
         <v>204</v>
       </c>
-      <c r="T23" s="0" t="s">
+      <c r="T23" t="s">
         <v>201</v>
       </c>
-      <c r="U23" s="0" t="s">
+      <c r="U23" t="s">
         <v>202</v>
       </c>
-      <c r="W23" s="0" t="s">
+      <c r="W23" t="s">
         <v>205</v>
       </c>
-      <c r="X23" s="0" t="s">
+      <c r="X23" t="s">
         <v>206</v>
       </c>
-      <c r="Z23" s="0" t="s">
+      <c r="Z23" t="s">
         <v>201</v>
       </c>
-      <c r="AA23" s="0" t="s">
+      <c r="AA23" t="s">
         <v>202</v>
       </c>
-      <c r="AC23" s="0" t="s">
+      <c r="AC23" t="s">
         <v>201</v>
       </c>
-      <c r="AD23" s="0" t="s">
+      <c r="AD23" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>208</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="3">
         <v>49</v>
       </c>
-      <c r="E24" s="3" t="n">
+      <c r="E24" s="3">
         <v>17</v>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="3">
         <v>0</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="0" t="s">
+      <c r="H24" t="s">
         <v>209</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" t="s">
         <v>210</v>
       </c>
-      <c r="K24" s="0" t="s">
+      <c r="K24" t="s">
         <v>209</v>
       </c>
-      <c r="L24" s="0" t="s">
+      <c r="L24" t="s">
         <v>210</v>
       </c>
-      <c r="N24" s="0" t="s">
+      <c r="N24" t="s">
         <v>209</v>
       </c>
-      <c r="O24" s="0" t="s">
+      <c r="O24" t="s">
         <v>210</v>
       </c>
-      <c r="Q24" s="0" t="s">
+      <c r="Q24" t="s">
         <v>211</v>
       </c>
-      <c r="R24" s="0" t="s">
+      <c r="R24" t="s">
         <v>212</v>
       </c>
-      <c r="T24" s="0" t="s">
+      <c r="T24" t="s">
         <v>209</v>
       </c>
-      <c r="U24" s="0" t="s">
+      <c r="U24" t="s">
         <v>210</v>
       </c>
-      <c r="W24" s="0" t="s">
+      <c r="W24" t="s">
         <v>213</v>
       </c>
-      <c r="X24" s="0" t="s">
+      <c r="X24" t="s">
         <v>214</v>
       </c>
-      <c r="Z24" s="0" t="s">
+      <c r="Z24" t="s">
         <v>209</v>
       </c>
-      <c r="AA24" s="0" t="s">
+      <c r="AA24" t="s">
         <v>210</v>
       </c>
-      <c r="AC24" s="0" t="s">
+      <c r="AC24" t="s">
         <v>209</v>
       </c>
-      <c r="AD24" s="0" t="s">
+      <c r="AD24" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>216</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>217</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="3">
         <v>47</v>
       </c>
-      <c r="E25" s="3" t="n">
+      <c r="E25" s="3">
         <v>19</v>
       </c>
-      <c r="F25" s="3" t="n">
+      <c r="F25" s="3">
         <v>0</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="0" t="s">
+      <c r="H25" t="s">
         <v>64</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="I25" t="s">
         <v>65</v>
       </c>
-      <c r="K25" s="0" t="s">
+      <c r="K25" t="s">
         <v>64</v>
       </c>
-      <c r="L25" s="0" t="s">
+      <c r="L25" t="s">
         <v>65</v>
       </c>
-      <c r="N25" s="0" t="s">
+      <c r="N25" t="s">
         <v>64</v>
       </c>
-      <c r="O25" s="0" t="s">
+      <c r="O25" t="s">
         <v>65</v>
       </c>
-      <c r="Q25" s="0" t="s">
+      <c r="Q25" t="s">
         <v>66</v>
       </c>
-      <c r="R25" s="0" t="s">
+      <c r="R25" t="s">
         <v>67</v>
       </c>
-      <c r="T25" s="0" t="s">
+      <c r="T25" t="s">
         <v>64</v>
       </c>
-      <c r="U25" s="0" t="s">
+      <c r="U25" t="s">
         <v>65</v>
       </c>
-      <c r="W25" s="0" t="s">
+      <c r="W25" t="s">
         <v>68</v>
       </c>
-      <c r="X25" s="0" t="s">
+      <c r="X25" t="s">
         <v>69</v>
       </c>
-      <c r="Z25" s="0" t="s">
+      <c r="Z25" t="s">
         <v>64</v>
       </c>
-      <c r="AA25" s="0" t="s">
+      <c r="AA25" t="s">
         <v>65</v>
       </c>
-      <c r="AC25" s="0" t="s">
+      <c r="AC25" t="s">
         <v>64</v>
       </c>
-      <c r="AD25" s="0" t="s">
+      <c r="AD25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>219</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="3">
         <v>43</v>
       </c>
-      <c r="E26" s="3" t="n">
+      <c r="E26" s="3">
         <v>12</v>
       </c>
-      <c r="F26" s="3" t="n">
+      <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="0" t="s">
+      <c r="H26" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" t="s">
         <v>221</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="K26" t="s">
         <v>220</v>
       </c>
-      <c r="L26" s="0" t="s">
+      <c r="L26" t="s">
         <v>221</v>
       </c>
-      <c r="N26" s="0" t="s">
+      <c r="N26" t="s">
         <v>220</v>
       </c>
-      <c r="O26" s="0" t="s">
+      <c r="O26" t="s">
         <v>221</v>
       </c>
-      <c r="Q26" s="0" t="s">
+      <c r="Q26" t="s">
         <v>222</v>
       </c>
-      <c r="R26" s="0" t="s">
+      <c r="R26" t="s">
         <v>223</v>
       </c>
-      <c r="T26" s="0" t="s">
+      <c r="T26" t="s">
         <v>220</v>
       </c>
-      <c r="U26" s="0" t="s">
+      <c r="U26" t="s">
         <v>221</v>
       </c>
-      <c r="W26" s="0" t="s">
+      <c r="W26" t="s">
         <v>224</v>
       </c>
-      <c r="X26" s="0" t="s">
+      <c r="X26" t="s">
         <v>225</v>
       </c>
-      <c r="Z26" s="0" t="s">
+      <c r="Z26" t="s">
         <v>220</v>
       </c>
-      <c r="AA26" s="0" t="s">
+      <c r="AA26" t="s">
         <v>221</v>
       </c>
-      <c r="AC26" s="0" t="s">
+      <c r="AC26" t="s">
         <v>220</v>
       </c>
-      <c r="AD26" s="0" t="s">
+      <c r="AD26" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>227</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" t="s">
         <v>228</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="3">
         <v>60</v>
       </c>
-      <c r="E27" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="F27" s="3" t="n">
-        <v>0</v>
+      <c r="E27" s="3">
+        <v>16</v>
+      </c>
+      <c r="F27" s="3">
+        <v>3</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="0" t="s">
+      <c r="H27" t="s">
         <v>81</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I27" t="s">
         <v>82</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="K27" t="s">
         <v>81</v>
       </c>
-      <c r="L27" s="0" t="s">
+      <c r="L27" t="s">
         <v>82</v>
       </c>
-      <c r="N27" s="0" t="s">
+      <c r="N27" t="s">
         <v>81</v>
       </c>
-      <c r="O27" s="0" t="s">
+      <c r="O27" t="s">
         <v>82</v>
       </c>
-      <c r="Q27" s="0" t="s">
+      <c r="Q27" t="s">
         <v>83</v>
       </c>
-      <c r="R27" s="0" t="s">
+      <c r="R27" t="s">
         <v>84</v>
       </c>
-      <c r="T27" s="0" t="s">
+      <c r="T27" t="s">
         <v>81</v>
       </c>
-      <c r="U27" s="0" t="s">
+      <c r="U27" t="s">
         <v>82</v>
       </c>
-      <c r="W27" s="0" t="s">
+      <c r="W27" t="s">
         <v>85</v>
       </c>
-      <c r="X27" s="0" t="s">
+      <c r="X27" t="s">
         <v>86</v>
       </c>
-      <c r="Z27" s="0" t="s">
+      <c r="Z27" t="s">
         <v>81</v>
       </c>
-      <c r="AA27" s="0" t="s">
+      <c r="AA27" t="s">
         <v>82</v>
       </c>
-      <c r="AC27" s="0" t="s">
+      <c r="AC27" t="s">
         <v>81</v>
       </c>
-      <c r="AD27" s="0" t="s">
+      <c r="AD27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>230</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>231</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="3">
         <v>65</v>
       </c>
-      <c r="E28" s="3" t="n">
+      <c r="E28" s="3">
         <v>10</v>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="3">
         <v>0</v>
       </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="0" t="s">
+      <c r="H28" t="s">
         <v>90</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" t="s">
         <v>91</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="K28" t="s">
         <v>90</v>
       </c>
-      <c r="L28" s="0" t="s">
+      <c r="L28" t="s">
         <v>91</v>
       </c>
-      <c r="N28" s="0" t="s">
+      <c r="N28" t="s">
         <v>90</v>
       </c>
-      <c r="O28" s="0" t="s">
+      <c r="O28" t="s">
         <v>91</v>
       </c>
-      <c r="Q28" s="0" t="s">
+      <c r="Q28" t="s">
         <v>92</v>
       </c>
-      <c r="R28" s="0" t="s">
+      <c r="R28" t="s">
         <v>93</v>
       </c>
-      <c r="T28" s="0" t="s">
+      <c r="T28" t="s">
         <v>90</v>
       </c>
-      <c r="U28" s="0" t="s">
+      <c r="U28" t="s">
         <v>91</v>
       </c>
-      <c r="W28" s="0" t="s">
+      <c r="W28" t="s">
         <v>94</v>
       </c>
-      <c r="X28" s="0" t="s">
+      <c r="X28" t="s">
         <v>95</v>
       </c>
-      <c r="Z28" s="0" t="s">
+      <c r="Z28" t="s">
         <v>90</v>
       </c>
-      <c r="AA28" s="0" t="s">
+      <c r="AA28" t="s">
         <v>91</v>
       </c>
-      <c r="AC28" s="0" t="s">
+      <c r="AC28" t="s">
         <v>90</v>
       </c>
-      <c r="AD28" s="0" t="s">
+      <c r="AD28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" t="s">
         <v>233</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="3">
         <v>68</v>
       </c>
-      <c r="E29" s="3" t="n">
+      <c r="E29" s="3">
         <v>10</v>
       </c>
-      <c r="F29" s="3" t="n">
+      <c r="F29" s="3">
         <v>0</v>
       </c>
       <c r="G29" s="3"/>
-      <c r="H29" s="0" t="s">
+      <c r="H29" t="s">
         <v>234</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="I29" t="s">
         <v>235</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="K29" t="s">
         <v>234</v>
       </c>
-      <c r="L29" s="0" t="s">
+      <c r="L29" t="s">
         <v>235</v>
       </c>
-      <c r="N29" s="0" t="s">
+      <c r="N29" t="s">
         <v>234</v>
       </c>
-      <c r="O29" s="0" t="s">
+      <c r="O29" t="s">
         <v>235</v>
       </c>
-      <c r="Q29" s="0" t="s">
+      <c r="Q29" t="s">
         <v>236</v>
       </c>
-      <c r="R29" s="0" t="s">
+      <c r="R29" t="s">
         <v>237</v>
       </c>
-      <c r="T29" s="0" t="s">
+      <c r="T29" t="s">
         <v>234</v>
       </c>
-      <c r="U29" s="0" t="s">
+      <c r="U29" t="s">
         <v>235</v>
       </c>
-      <c r="W29" s="0" t="s">
+      <c r="W29" t="s">
         <v>238</v>
       </c>
-      <c r="X29" s="0" t="s">
+      <c r="X29" t="s">
         <v>239</v>
       </c>
-      <c r="Z29" s="0" t="s">
+      <c r="Z29" t="s">
         <v>234</v>
       </c>
-      <c r="AA29" s="0" t="s">
+      <c r="AA29" t="s">
         <v>235</v>
       </c>
-      <c r="AC29" s="0" t="s">
+      <c r="AC29" t="s">
         <v>234</v>
       </c>
-      <c r="AD29" s="0" t="s">
+      <c r="AD29" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" t="s">
         <v>241</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="3">
         <v>72</v>
       </c>
-      <c r="E30" s="3" t="n">
+      <c r="E30" s="3">
         <v>27</v>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="F30" s="3">
         <v>1</v>
       </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="0" t="s">
+      <c r="H30" t="s">
         <v>242</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="I30" t="s">
         <v>243</v>
       </c>
-      <c r="K30" s="0" t="s">
+      <c r="K30" t="s">
         <v>242</v>
       </c>
-      <c r="L30" s="0" t="s">
+      <c r="L30" t="s">
         <v>243</v>
       </c>
-      <c r="N30" s="0" t="s">
+      <c r="N30" t="s">
         <v>242</v>
       </c>
-      <c r="O30" s="0" t="s">
+      <c r="O30" t="s">
         <v>243</v>
       </c>
-      <c r="Q30" s="0" t="s">
+      <c r="Q30" t="s">
         <v>244</v>
       </c>
-      <c r="R30" s="0" t="s">
+      <c r="R30" t="s">
         <v>245</v>
       </c>
-      <c r="T30" s="0" t="s">
+      <c r="T30" t="s">
         <v>242</v>
       </c>
-      <c r="U30" s="0" t="s">
+      <c r="U30" t="s">
         <v>243</v>
       </c>
-      <c r="W30" s="0" t="s">
+      <c r="W30" t="s">
         <v>246</v>
       </c>
-      <c r="X30" s="0" t="s">
+      <c r="X30" t="s">
         <v>247</v>
       </c>
-      <c r="Z30" s="0" t="s">
+      <c r="Z30" t="s">
         <v>242</v>
       </c>
-      <c r="AA30" s="0" t="s">
+      <c r="AA30" t="s">
         <v>243</v>
       </c>
-      <c r="AC30" s="0" t="s">
+      <c r="AC30" t="s">
         <v>242</v>
       </c>
-      <c r="AD30" s="0" t="s">
+      <c r="AD30" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" t="s">
         <v>249</v>
       </c>
-      <c r="D31" s="3" t="n">
+      <c r="D31" s="3">
         <v>59</v>
       </c>
-      <c r="E31" s="3" t="n">
+      <c r="E31" s="3">
         <v>21</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="0" t="s">
+      <c r="H31" t="s">
         <v>250</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="I31" t="s">
         <v>251</v>
       </c>
-      <c r="K31" s="0" t="s">
+      <c r="K31" t="s">
         <v>250</v>
       </c>
-      <c r="L31" s="0" t="s">
+      <c r="L31" t="s">
         <v>251</v>
       </c>
-      <c r="N31" s="0" t="s">
+      <c r="N31" t="s">
         <v>250</v>
       </c>
-      <c r="O31" s="0" t="s">
+      <c r="O31" t="s">
         <v>251</v>
       </c>
-      <c r="Q31" s="0" t="s">
+      <c r="Q31" t="s">
         <v>252</v>
       </c>
-      <c r="R31" s="0" t="s">
+      <c r="R31" t="s">
         <v>253</v>
       </c>
-      <c r="T31" s="0" t="s">
+      <c r="T31" t="s">
         <v>250</v>
       </c>
-      <c r="U31" s="0" t="s">
+      <c r="U31" t="s">
         <v>251</v>
       </c>
-      <c r="W31" s="0" t="s">
+      <c r="W31" t="s">
         <v>254</v>
       </c>
-      <c r="X31" s="0" t="s">
+      <c r="X31" t="s">
         <v>255</v>
       </c>
-      <c r="Z31" s="0" t="s">
+      <c r="Z31" t="s">
         <v>250</v>
       </c>
-      <c r="AA31" s="0" t="s">
+      <c r="AA31" t="s">
         <v>251</v>
       </c>
-      <c r="AC31" s="0" t="s">
+      <c r="AC31" t="s">
         <v>250</v>
       </c>
-      <c r="AD31" s="0" t="s">
+      <c r="AD31" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" t="s">
         <v>257</v>
       </c>
-      <c r="D32" s="3" t="n">
+      <c r="D32" s="3">
         <v>51</v>
       </c>
-      <c r="E32" s="3" t="n">
+      <c r="E32" s="3">
         <v>14</v>
       </c>
-      <c r="F32" s="3" t="n">
+      <c r="F32" s="3">
         <v>0</v>
       </c>
       <c r="G32" s="3"/>
-      <c r="H32" s="0" t="s">
+      <c r="H32" t="s">
         <v>258</v>
       </c>
-      <c r="I32" s="0" t="s">
+      <c r="I32" t="s">
         <v>259</v>
       </c>
-      <c r="K32" s="0" t="s">
+      <c r="K32" t="s">
         <v>258</v>
       </c>
-      <c r="L32" s="0" t="s">
+      <c r="L32" t="s">
         <v>259</v>
       </c>
-      <c r="N32" s="0" t="s">
+      <c r="N32" t="s">
         <v>258</v>
       </c>
-      <c r="O32" s="0" t="s">
+      <c r="O32" t="s">
         <v>259</v>
       </c>
-      <c r="Q32" s="0" t="s">
+      <c r="Q32" t="s">
         <v>260</v>
       </c>
-      <c r="R32" s="0" t="s">
+      <c r="R32" t="s">
         <v>261</v>
       </c>
-      <c r="T32" s="0" t="s">
+      <c r="T32" t="s">
         <v>258</v>
       </c>
-      <c r="U32" s="0" t="s">
+      <c r="U32" t="s">
         <v>259</v>
       </c>
-      <c r="W32" s="0" t="s">
+      <c r="W32" t="s">
         <v>262</v>
       </c>
-      <c r="X32" s="0" t="s">
+      <c r="X32" t="s">
         <v>263</v>
       </c>
-      <c r="Z32" s="0" t="s">
+      <c r="Z32" t="s">
         <v>258</v>
       </c>
-      <c r="AA32" s="0" t="s">
+      <c r="AA32" t="s">
         <v>259</v>
       </c>
-      <c r="AC32" s="0" t="s">
+      <c r="AC32" t="s">
         <v>258</v>
       </c>
-      <c r="AD32" s="0" t="s">
+      <c r="AD32" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" t="s">
         <v>265</v>
       </c>
-      <c r="D33" s="3" t="n">
+      <c r="D33" s="3">
         <v>55</v>
       </c>
-      <c r="E33" s="3" t="n">
+      <c r="E33" s="3">
         <v>18</v>
       </c>
-      <c r="F33" s="3" t="n">
+      <c r="F33" s="3">
         <v>7</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="0" t="s">
+      <c r="H33" t="s">
         <v>266</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="I33" t="s">
         <v>267</v>
       </c>
-      <c r="K33" s="0" t="s">
+      <c r="K33" t="s">
         <v>266</v>
       </c>
-      <c r="L33" s="0" t="s">
+      <c r="L33" t="s">
         <v>267</v>
       </c>
-      <c r="N33" s="0" t="s">
+      <c r="N33" t="s">
         <v>266</v>
       </c>
-      <c r="O33" s="0" t="s">
+      <c r="O33" t="s">
         <v>267</v>
       </c>
-      <c r="Q33" s="0" t="s">
+      <c r="Q33" t="s">
         <v>268</v>
       </c>
-      <c r="R33" s="0" t="s">
+      <c r="R33" t="s">
         <v>269</v>
       </c>
-      <c r="T33" s="0" t="s">
+      <c r="T33" t="s">
         <v>266</v>
       </c>
-      <c r="U33" s="0" t="s">
+      <c r="U33" t="s">
         <v>267</v>
       </c>
-      <c r="W33" s="0" t="s">
+      <c r="W33" t="s">
         <v>270</v>
       </c>
-      <c r="X33" s="0" t="s">
+      <c r="X33" t="s">
         <v>271</v>
       </c>
-      <c r="Z33" s="0" t="s">
+      <c r="Z33" t="s">
         <v>266</v>
       </c>
-      <c r="AA33" s="0" t="s">
+      <c r="AA33" t="s">
         <v>267</v>
       </c>
-      <c r="AC33" s="0" t="s">
+      <c r="AC33" t="s">
         <v>266</v>
       </c>
-      <c r="AD33" s="0" t="s">
+      <c r="AD33" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>272</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>273</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" t="s">
         <v>273</v>
       </c>
-      <c r="D34" s="3" t="n">
+      <c r="D34" s="3">
         <v>3</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" t="s">
         <v>273</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" t="s">
         <v>273</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="H34" t="s">
         <v>274</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="I34" t="s">
         <v>273</v>
       </c>
-      <c r="K34" s="0" t="s">
+      <c r="K34" t="s">
         <v>274</v>
       </c>
-      <c r="L34" s="0" t="s">
+      <c r="L34" t="s">
         <v>273</v>
       </c>
-      <c r="N34" s="0" t="s">
+      <c r="N34" t="s">
         <v>274</v>
       </c>
-      <c r="O34" s="0" t="s">
+      <c r="O34" t="s">
         <v>273</v>
       </c>
-      <c r="Q34" s="0" t="s">
+      <c r="Q34" t="s">
         <v>275</v>
       </c>
-      <c r="R34" s="0" t="s">
+      <c r="R34" t="s">
         <v>273</v>
       </c>
-      <c r="T34" s="0" t="s">
+      <c r="T34" t="s">
         <v>274</v>
       </c>
-      <c r="U34" s="0" t="s">
+      <c r="U34" t="s">
         <v>273</v>
       </c>
-      <c r="W34" s="0" t="s">
+      <c r="W34" t="s">
         <v>276</v>
       </c>
-      <c r="X34" s="0" t="s">
+      <c r="X34" t="s">
         <v>273</v>
       </c>
-      <c r="Z34" s="0" t="s">
+      <c r="Z34" t="s">
         <v>274</v>
       </c>
-      <c r="AA34" s="0" t="s">
+      <c r="AA34" t="s">
         <v>273</v>
       </c>
-      <c r="AC34" s="0" t="s">
+      <c r="AC34" t="s">
         <v>274</v>
       </c>
-      <c r="AD34" s="0" t="s">
+      <c r="AD34" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>277</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>273</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" t="s">
         <v>273</v>
       </c>
-      <c r="D35" s="3" t="n">
+      <c r="D35" s="3">
         <v>69</v>
       </c>
-      <c r="E35" s="4" t="n">
+      <c r="E35" s="4">
         <v>4</v>
       </c>
-      <c r="F35" s="4" t="n">
+      <c r="F35" s="4">
         <v>12</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="H35" t="s">
         <v>278</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="I35" t="s">
         <v>279</v>
       </c>
-      <c r="K35" s="0" t="s">
+      <c r="K35" t="s">
         <v>278</v>
       </c>
-      <c r="L35" s="0" t="s">
+      <c r="L35" t="s">
         <v>279</v>
       </c>
-      <c r="N35" s="0" t="s">
+      <c r="N35" t="s">
         <v>278</v>
       </c>
-      <c r="O35" s="0" t="s">
+      <c r="O35" t="s">
         <v>279</v>
       </c>
-      <c r="Q35" s="0" t="s">
+      <c r="Q35" t="s">
         <v>280</v>
       </c>
-      <c r="R35" s="0" t="s">
+      <c r="R35" t="s">
         <v>281</v>
       </c>
-      <c r="T35" s="0" t="s">
+      <c r="T35" t="s">
         <v>278</v>
       </c>
-      <c r="U35" s="0" t="s">
+      <c r="U35" t="s">
         <v>279</v>
       </c>
-      <c r="W35" s="0" t="s">
+      <c r="W35" t="s">
         <v>282</v>
       </c>
-      <c r="X35" s="0" t="s">
+      <c r="X35" t="s">
         <v>283</v>
       </c>
-      <c r="Z35" s="0" t="s">
+      <c r="Z35" t="s">
         <v>278</v>
       </c>
-      <c r="AA35" s="0" t="s">
+      <c r="AA35" t="s">
         <v>279</v>
       </c>
-      <c r="AC35" s="0" t="s">
+      <c r="AC35" t="s">
         <v>278</v>
       </c>
-      <c r="AD35" s="0" t="s">
+      <c r="AD35" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>284</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>273</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" t="s">
         <v>273</v>
       </c>
-      <c r="D36" s="3" t="n">
+      <c r="D36" s="3">
         <v>9</v>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="4">
         <v>1</v>
       </c>
-      <c r="F36" s="4" t="n">
+      <c r="F36" s="4">
         <v>2</v>
       </c>
-      <c r="H36" s="0" t="s">
+      <c r="H36" t="s">
         <v>285</v>
       </c>
-      <c r="I36" s="0" t="s">
+      <c r="I36" t="s">
         <v>286</v>
       </c>
-      <c r="K36" s="0" t="s">
+      <c r="K36" t="s">
         <v>285</v>
       </c>
-      <c r="L36" s="0" t="s">
+      <c r="L36" t="s">
         <v>286</v>
       </c>
-      <c r="N36" s="0" t="s">
+      <c r="N36" t="s">
         <v>285</v>
       </c>
-      <c r="O36" s="0" t="s">
+      <c r="O36" t="s">
         <v>286</v>
       </c>
-      <c r="Q36" s="0" t="s">
+      <c r="Q36" t="s">
         <v>287</v>
       </c>
-      <c r="R36" s="0" t="s">
+      <c r="R36" t="s">
         <v>288</v>
       </c>
-      <c r="T36" s="0" t="s">
+      <c r="T36" t="s">
         <v>285</v>
       </c>
-      <c r="U36" s="0" t="s">
+      <c r="U36" t="s">
         <v>286</v>
       </c>
-      <c r="W36" s="0" t="s">
+      <c r="W36" t="s">
         <v>289</v>
       </c>
-      <c r="X36" s="0" t="s">
+      <c r="X36" t="s">
         <v>290</v>
       </c>
-      <c r="Z36" s="0" t="s">
+      <c r="Z36" t="s">
         <v>285</v>
       </c>
-      <c r="AA36" s="0" t="s">
+      <c r="AA36" t="s">
         <v>286</v>
       </c>
-      <c r="AC36" s="0" t="s">
+      <c r="AC36" t="s">
         <v>285</v>
       </c>
-      <c r="AD36" s="0" t="s">
+      <c r="AD36" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>291</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>273</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" t="s">
         <v>273</v>
       </c>
-      <c r="D37" s="3" t="n">
+      <c r="D37" s="3">
         <v>20</v>
       </c>
-      <c r="E37" s="4" t="n">
+      <c r="E37" s="4">
         <v>1</v>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="F37" s="4">
         <v>2</v>
       </c>
-      <c r="H37" s="0" t="s">
+      <c r="H37" t="s">
         <v>292</v>
       </c>
-      <c r="I37" s="0" t="s">
+      <c r="I37" t="s">
         <v>293</v>
       </c>
-      <c r="K37" s="0" t="s">
+      <c r="K37" t="s">
         <v>292</v>
       </c>
-      <c r="L37" s="0" t="s">
+      <c r="L37" t="s">
         <v>293</v>
       </c>
-      <c r="N37" s="0" t="s">
+      <c r="N37" t="s">
         <v>292</v>
       </c>
-      <c r="O37" s="0" t="s">
+      <c r="O37" t="s">
         <v>293</v>
       </c>
-      <c r="Q37" s="0" t="s">
+      <c r="Q37" t="s">
         <v>294</v>
       </c>
-      <c r="R37" s="0" t="s">
+      <c r="R37" t="s">
         <v>295</v>
       </c>
-      <c r="T37" s="0" t="s">
+      <c r="T37" t="s">
         <v>292</v>
       </c>
-      <c r="U37" s="0" t="s">
+      <c r="U37" t="s">
         <v>293</v>
       </c>
-      <c r="W37" s="0" t="s">
+      <c r="W37" t="s">
         <v>296</v>
       </c>
-      <c r="X37" s="0" t="s">
+      <c r="X37" t="s">
         <v>297</v>
       </c>
-      <c r="Z37" s="0" t="s">
+      <c r="Z37" t="s">
         <v>292</v>
       </c>
-      <c r="AA37" s="0" t="s">
+      <c r="AA37" t="s">
         <v>293</v>
       </c>
-      <c r="AC37" s="0" t="s">
+      <c r="AC37" t="s">
         <v>292</v>
       </c>
-      <c r="AD37" s="0" t="s">
+      <c r="AD37" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>298</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>273</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" t="s">
         <v>273</v>
       </c>
-      <c r="D38" s="3" t="n">
+      <c r="D38" s="3">
         <v>23</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" t="s">
         <v>273</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" t="s">
         <v>273</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="H38" t="s">
         <v>299</v>
       </c>
-      <c r="I38" s="0" t="s">
+      <c r="I38" t="s">
         <v>273</v>
       </c>
-      <c r="K38" s="0" t="s">
+      <c r="K38" t="s">
         <v>299</v>
       </c>
-      <c r="L38" s="0" t="s">
+      <c r="L38" t="s">
         <v>273</v>
       </c>
-      <c r="N38" s="0" t="s">
+      <c r="N38" t="s">
         <v>299</v>
       </c>
-      <c r="O38" s="0" t="s">
+      <c r="O38" t="s">
         <v>273</v>
       </c>
-      <c r="Q38" s="0" t="s">
+      <c r="Q38" t="s">
         <v>300</v>
       </c>
-      <c r="R38" s="0" t="s">
+      <c r="R38" t="s">
         <v>273</v>
       </c>
-      <c r="T38" s="0" t="s">
+      <c r="T38" t="s">
         <v>299</v>
       </c>
-      <c r="U38" s="0" t="s">
+      <c r="U38" t="s">
         <v>273</v>
       </c>
-      <c r="W38" s="0" t="s">
+      <c r="W38" t="s">
         <v>301</v>
       </c>
-      <c r="X38" s="0" t="s">
+      <c r="X38" t="s">
         <v>273</v>
       </c>
-      <c r="Z38" s="0" t="s">
+      <c r="Z38" t="s">
         <v>299</v>
       </c>
-      <c r="AA38" s="0" t="s">
+      <c r="AA38" t="s">
         <v>273</v>
       </c>
-      <c r="AC38" s="0" t="s">
+      <c r="AC38" t="s">
         <v>299</v>
       </c>
-      <c r="AD38" s="0" t="s">
+      <c r="AD38" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>302</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>273</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" t="s">
         <v>273</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="3">
         <v>30</v>
       </c>
-      <c r="E39" s="4" t="n">
+      <c r="E39" s="4">
         <v>5</v>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="F39" s="4">
         <v>2</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="H39" t="s">
         <v>303</v>
       </c>
-      <c r="I39" s="0" t="s">
+      <c r="I39" t="s">
         <v>304</v>
       </c>
-      <c r="K39" s="0" t="s">
+      <c r="K39" t="s">
         <v>303</v>
       </c>
-      <c r="L39" s="0" t="s">
+      <c r="L39" t="s">
         <v>304</v>
       </c>
-      <c r="N39" s="0" t="s">
+      <c r="N39" t="s">
         <v>303</v>
       </c>
-      <c r="O39" s="0" t="s">
+      <c r="O39" t="s">
         <v>304</v>
       </c>
-      <c r="Q39" s="0" t="s">
+      <c r="Q39" t="s">
         <v>305</v>
       </c>
-      <c r="R39" s="0" t="s">
+      <c r="R39" t="s">
         <v>306</v>
       </c>
-      <c r="T39" s="0" t="s">
+      <c r="T39" t="s">
         <v>303</v>
       </c>
-      <c r="U39" s="0" t="s">
+      <c r="U39" t="s">
         <v>304</v>
       </c>
-      <c r="W39" s="0" t="s">
+      <c r="W39" t="s">
         <v>307</v>
       </c>
-      <c r="X39" s="0" t="s">
+      <c r="X39" t="s">
         <v>308</v>
       </c>
-      <c r="Z39" s="0" t="s">
+      <c r="Z39" t="s">
         <v>303</v>
       </c>
-      <c r="AA39" s="0" t="s">
+      <c r="AA39" t="s">
         <v>304</v>
       </c>
-      <c r="AC39" s="0" t="s">
+      <c r="AC39" t="s">
         <v>303</v>
       </c>
-      <c r="AD39" s="0" t="s">
+      <c r="AD39" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>309</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>273</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" t="s">
         <v>273</v>
       </c>
-      <c r="D40" s="3" t="n">
+      <c r="D40" s="3">
         <v>12</v>
       </c>
-      <c r="E40" s="4" t="n">
+      <c r="E40" s="4">
         <v>8</v>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="4">
         <v>1</v>
       </c>
-      <c r="H40" s="0" t="s">
+      <c r="H40" t="s">
         <v>310</v>
       </c>
-      <c r="I40" s="0" t="s">
+      <c r="I40" t="s">
         <v>311</v>
       </c>
-      <c r="K40" s="0" t="s">
+      <c r="K40" t="s">
         <v>310</v>
       </c>
-      <c r="L40" s="0" t="s">
+      <c r="L40" t="s">
         <v>311</v>
       </c>
-      <c r="N40" s="0" t="s">
+      <c r="N40" t="s">
         <v>310</v>
       </c>
-      <c r="O40" s="0" t="s">
+      <c r="O40" t="s">
         <v>311</v>
       </c>
-      <c r="Q40" s="0" t="s">
+      <c r="Q40" t="s">
         <v>312</v>
       </c>
-      <c r="R40" s="0" t="s">
+      <c r="R40" t="s">
         <v>313</v>
       </c>
-      <c r="T40" s="0" t="s">
+      <c r="T40" t="s">
         <v>310</v>
       </c>
-      <c r="U40" s="0" t="s">
+      <c r="U40" t="s">
         <v>311</v>
       </c>
-      <c r="W40" s="0" t="s">
+      <c r="W40" t="s">
         <v>314</v>
       </c>
-      <c r="X40" s="0" t="s">
+      <c r="X40" t="s">
         <v>315</v>
       </c>
-      <c r="Z40" s="0" t="s">
+      <c r="Z40" t="s">
         <v>310</v>
       </c>
-      <c r="AA40" s="0" t="s">
+      <c r="AA40" t="s">
         <v>311</v>
       </c>
-      <c r="AC40" s="0" t="s">
+      <c r="AC40" t="s">
         <v>310</v>
       </c>
-      <c r="AD40" s="0" t="s">
+      <c r="AD40" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>316</v>
       </c>
-      <c r="D42" s="4" t="n">
+      <c r="D42" s="4">
         <v>1916</v>
       </c>
-      <c r="E42" s="4" t="n">
+      <c r="E42" s="4">
         <v>546</v>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="4">
         <v>51</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>317</v>
       </c>
-      <c r="D43" s="4" t="n">
+      <c r="D43" s="4">
         <v>3832</v>
       </c>
-      <c r="E43" s="4" t="n">
+      <c r="E43" s="4">
         <v>1092</v>
       </c>
-      <c r="F43" s="4" t="n">
+      <c r="F43" s="4">
         <v>153</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>318</v>
       </c>
-      <c r="D44" s="4" t="n">
+      <c r="D44" s="4">
         <v>3832</v>
       </c>
-      <c r="E44" s="4" t="n">
+      <c r="E44" s="4">
         <v>1245</v>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="4">
         <v>1245</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.77551020408163"/>
+    <col min="1" max="1025" width="8.77734375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.77551020408163"/>
+    <col min="1" max="1025" width="8.77734375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>